<commit_message>
solved merged cells issue in excel
</commit_message>
<xml_diff>
--- a/data-stories/COVID-19/PPP-data.xlsx
+++ b/data-stories/COVID-19/PPP-data.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/philiplindsay/Documents/Classes/Psych/Storytelling/git/data-stories/COVID-19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{64A4D233-B8B7-3444-82FD-604D97718DD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A37AB3A8-3219-7943-8C02-5A8C4F9A8F31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{3A25139B-F7C9-2F40-9F60-A201A3DE4647}"/>
   </bookViews>
   <sheets>
-    <sheet name="States and Territories" sheetId="1" r:id="rId1"/>
-    <sheet name="Loan Size" sheetId="2" r:id="rId2"/>
-    <sheet name="Industry by NAICS Subsector" sheetId="3" r:id="rId3"/>
+    <sheet name="states_and_territories" sheetId="1" r:id="rId1"/>
+    <sheet name="loan_size" sheetId="2" r:id="rId2"/>
+    <sheet name="industry_by_naics_subsector" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -208,9 +208,6 @@
     <t xml:space="preserve">WY </t>
   </si>
   <si>
-    <t xml:space="preserve">Loan Size </t>
-  </si>
-  <si>
     <t xml:space="preserve">Approved Loans </t>
   </si>
   <si>
@@ -283,7 +280,10 @@
     <t>Approved Loans</t>
   </si>
   <si>
-    <t>Approved Amount</t>
+    <t>Lone Size</t>
+  </si>
+  <si>
+    <t>Approved Amounts</t>
   </si>
 </sst>
 </file>
@@ -349,24 +349,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="6" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="6" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="6" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="6" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -684,7 +683,7 @@
   <dimension ref="A1:H58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -694,42 +693,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="34" customHeight="1">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="C1" s="16" t="s">
+      <c r="B1" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="D1" s="10"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
+      <c r="D1" s="4"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="15">
+      <c r="B2" s="8">
         <v>4842</v>
       </c>
-      <c r="C2" s="14">
+      <c r="C2" s="7">
         <v>921927504</v>
       </c>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
     </row>
     <row r="3" spans="1:8" ht="16" customHeight="1">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B3" s="8">
         <v>27922</v>
       </c>
-      <c r="C3" s="14">
+      <c r="C3" s="7">
         <v>4862690120</v>
       </c>
       <c r="F3" s="1"/>
@@ -737,13 +736,13 @@
       <c r="H3" s="3"/>
     </row>
     <row r="4" spans="1:8" ht="16" customHeight="1">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="8">
         <v>21754</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="7">
         <v>2722726557</v>
       </c>
       <c r="F4" s="1"/>
@@ -751,13 +750,13 @@
       <c r="H4" s="3"/>
     </row>
     <row r="5" spans="1:8" ht="16" customHeight="1">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B5" s="6">
         <v>2</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="7">
         <v>419583</v>
       </c>
       <c r="F5" s="1"/>
@@ -765,13 +764,13 @@
       <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:8" ht="16" customHeight="1">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B6" s="8">
         <v>19280</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="7">
         <v>4846959062</v>
       </c>
       <c r="F6" s="1"/>
@@ -779,13 +778,13 @@
       <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:8" ht="16" customHeight="1">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="8">
         <v>112967</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="7">
         <v>33413693192</v>
       </c>
       <c r="F7" s="1"/>
@@ -793,13 +792,13 @@
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8" ht="16" customHeight="1">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="15">
+      <c r="B8" s="8">
         <v>41635</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="7">
         <v>7392960359</v>
       </c>
       <c r="F8" s="1"/>
@@ -807,13 +806,13 @@
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:8" ht="16" customHeight="1">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="15">
+      <c r="B9" s="8">
         <v>18435</v>
       </c>
-      <c r="C9" s="14">
+      <c r="C9" s="7">
         <v>4151934451</v>
       </c>
       <c r="F9" s="1"/>
@@ -821,13 +820,13 @@
       <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:8" ht="16" customHeight="1">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="15">
+      <c r="B10" s="8">
         <v>3253</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C10" s="7">
         <v>1247218727</v>
       </c>
       <c r="F10" s="1"/>
@@ -835,13 +834,13 @@
       <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:8" ht="16" customHeight="1">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="15">
+      <c r="B11" s="8">
         <v>5171</v>
       </c>
-      <c r="C11" s="14">
+      <c r="C11" s="7">
         <v>1090415848</v>
       </c>
       <c r="F11" s="1"/>
@@ -849,420 +848,420 @@
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:8" ht="16" customHeight="1">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="15">
+      <c r="B12" s="8">
         <v>88997</v>
       </c>
-      <c r="C12" s="14">
+      <c r="C12" s="7">
         <v>17863199837</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="16" customHeight="1">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="15">
+      <c r="B13" s="8">
         <v>48332</v>
       </c>
-      <c r="C13" s="14">
+      <c r="C13" s="7">
         <v>9464475442</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="16" customHeight="1">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="13">
+      <c r="B14" s="6">
         <v>508</v>
       </c>
-      <c r="C14" s="14">
+      <c r="C14" s="7">
         <v>102418346</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="16" customHeight="1">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="15">
+      <c r="B15" s="8">
         <v>11553</v>
       </c>
-      <c r="C15" s="14">
+      <c r="C15" s="7">
         <v>2046450982</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="16" customHeight="1">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="15">
+      <c r="B16" s="8">
         <v>29424</v>
       </c>
-      <c r="C16" s="14">
+      <c r="C16" s="7">
         <v>4315688444</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="16" customHeight="1">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="15">
+      <c r="B17" s="8">
         <v>13627</v>
       </c>
-      <c r="C17" s="14">
+      <c r="C17" s="7">
         <v>1850034026</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="16" customHeight="1">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="15">
+      <c r="B18" s="8">
         <v>69893</v>
       </c>
-      <c r="C18" s="14">
+      <c r="C18" s="7">
         <v>15972578071</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="16" customHeight="1">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="15">
+      <c r="B19" s="8">
         <v>35990</v>
       </c>
-      <c r="C19" s="14">
+      <c r="C19" s="7">
         <v>7491445351</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="16" customHeight="1">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="15">
+      <c r="B20" s="8">
         <v>26245</v>
       </c>
-      <c r="C20" s="14">
+      <c r="C20" s="7">
         <v>4288652108</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="16" customHeight="1">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="15">
+      <c r="B21" s="8">
         <v>23797</v>
       </c>
-      <c r="C21" s="14">
+      <c r="C21" s="7">
         <v>4149467684</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="16" customHeight="1">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="15">
+      <c r="B22" s="8">
         <v>26635</v>
       </c>
-      <c r="C22" s="14">
+      <c r="C22" s="7">
         <v>5100534501</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="16" customHeight="1">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="15">
+      <c r="B23" s="8">
         <v>46937</v>
       </c>
-      <c r="C23" s="14">
+      <c r="C23" s="7">
         <v>10360907178</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="16" customHeight="1">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="15">
+      <c r="B24" s="8">
         <v>26068</v>
       </c>
-      <c r="C24" s="14">
+      <c r="C24" s="7">
         <v>6537733687</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="16" customHeight="1">
-      <c r="A25" s="13" t="s">
+      <c r="A25" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="15">
+      <c r="B25" s="8">
         <v>14993</v>
       </c>
-      <c r="C25" s="14">
+      <c r="C25" s="7">
         <v>1944425549</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="16" customHeight="1">
-      <c r="A26" s="13" t="s">
+      <c r="A26" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="15">
+      <c r="B26" s="8">
         <v>43438</v>
       </c>
-      <c r="C26" s="14">
+      <c r="C26" s="7">
         <v>10381310070</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="16" customHeight="1">
-      <c r="A27" s="13" t="s">
+      <c r="A27" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="15">
+      <c r="B27" s="8">
         <v>46383</v>
       </c>
-      <c r="C27" s="14">
+      <c r="C27" s="7">
         <v>9014060040</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="16" customHeight="1">
-      <c r="A28" s="13" t="s">
+      <c r="A28" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="15">
+      <c r="B28" s="8">
         <v>46481</v>
       </c>
-      <c r="C28" s="14">
+      <c r="C28" s="7">
         <v>7547822023</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="16" customHeight="1">
-      <c r="A29" s="13" t="s">
+      <c r="A29" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="13">
+      <c r="B29" s="6">
         <v>56</v>
       </c>
-      <c r="C29" s="14">
+      <c r="C29" s="7">
         <v>12619835</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="16" customHeight="1">
-      <c r="A30" s="13" t="s">
+      <c r="A30" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="15">
+      <c r="B30" s="8">
         <v>20748</v>
       </c>
-      <c r="C30" s="14">
+      <c r="C30" s="7">
         <v>2481000606</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="16" customHeight="1">
-      <c r="A31" s="13" t="s">
+      <c r="A31" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="15">
+      <c r="B31" s="8">
         <v>13456</v>
       </c>
-      <c r="C31" s="14">
+      <c r="C31" s="7">
         <v>1470300136</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="16" customHeight="1">
-      <c r="A32" s="13" t="s">
+      <c r="A32" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="15">
+      <c r="B32" s="8">
         <v>39520</v>
       </c>
-      <c r="C32" s="14">
+      <c r="C32" s="7">
         <v>8005752270</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="16" customHeight="1">
-      <c r="A33" s="13" t="s">
+      <c r="A33" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="15">
+      <c r="B33" s="8">
         <v>11002</v>
       </c>
-      <c r="C33" s="14">
+      <c r="C33" s="7">
         <v>1548384035</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="16" customHeight="1">
-      <c r="A34" s="13" t="s">
+      <c r="A34" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="15">
+      <c r="B34" s="8">
         <v>23477</v>
       </c>
-      <c r="C34" s="14">
+      <c r="C34" s="7">
         <v>2988890489</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="16" customHeight="1">
-      <c r="A35" s="13" t="s">
+      <c r="A35" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="15">
+      <c r="B35" s="8">
         <v>11582</v>
       </c>
-      <c r="C35" s="14">
+      <c r="C35" s="7">
         <v>2006858477</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="16" customHeight="1">
-      <c r="A36" s="13" t="s">
+      <c r="A36" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="15">
+      <c r="B36" s="8">
         <v>33519</v>
       </c>
-      <c r="C36" s="14">
+      <c r="C36" s="7">
         <v>9527794260</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="16" customHeight="1">
-      <c r="A37" s="13" t="s">
+      <c r="A37" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B37" s="15">
+      <c r="B37" s="8">
         <v>8277</v>
       </c>
-      <c r="C37" s="14">
+      <c r="C37" s="7">
         <v>1424408711</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="16" customHeight="1">
-      <c r="A38" s="13" t="s">
+      <c r="A38" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B38" s="15">
+      <c r="B38" s="8">
         <v>8674</v>
       </c>
-      <c r="C38" s="14">
+      <c r="C38" s="7">
         <v>2013939889</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="16" customHeight="1">
-      <c r="A39" s="13" t="s">
+      <c r="A39" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B39" s="15">
+      <c r="B39" s="8">
         <v>81075</v>
       </c>
-      <c r="C39" s="14">
+      <c r="C39" s="7">
         <v>20345681101</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="16" customHeight="1">
-      <c r="A40" s="13" t="s">
+      <c r="A40" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B40" s="15">
+      <c r="B40" s="8">
         <v>59800</v>
       </c>
-      <c r="C40" s="14">
+      <c r="C40" s="7">
         <v>14108889927</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="16" customHeight="1">
-      <c r="A41" s="13" t="s">
+      <c r="A41" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B41" s="15">
+      <c r="B41" s="8">
         <v>35557</v>
       </c>
-      <c r="C41" s="14">
+      <c r="C41" s="7">
         <v>4615708450</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="16" customHeight="1">
-      <c r="A42" s="13" t="s">
+      <c r="A42" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B42" s="15">
+      <c r="B42" s="8">
         <v>18732</v>
       </c>
-      <c r="C42" s="14">
+      <c r="C42" s="7">
         <v>3806104476</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="16" customHeight="1">
-      <c r="A43" s="13" t="s">
+      <c r="A43" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B43" s="15">
+      <c r="B43" s="8">
         <v>69567</v>
       </c>
-      <c r="C43" s="14">
+      <c r="C43" s="7">
         <v>15697648689</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="16" customHeight="1">
-      <c r="A44" s="13" t="s">
+      <c r="A44" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B44" s="15">
+      <c r="B44" s="8">
         <v>2856</v>
       </c>
-      <c r="C44" s="14">
+      <c r="C44" s="7">
         <v>658573638</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="16" customHeight="1">
-      <c r="A45" s="13" t="s">
+      <c r="A45" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B45" s="15">
+      <c r="B45" s="8">
         <v>7732</v>
       </c>
-      <c r="C45" s="14">
+      <c r="C45" s="7">
         <v>1335777801</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="16" customHeight="1">
-      <c r="A46" s="13" t="s">
+      <c r="A46" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B46" s="15">
+      <c r="B46" s="8">
         <v>22933</v>
       </c>
-      <c r="C46" s="14">
+      <c r="C46" s="7">
         <v>3807578397</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="16" customHeight="1">
-      <c r="A47" s="13" t="s">
+      <c r="A47" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B47" s="15">
+      <c r="B47" s="8">
         <v>11324</v>
       </c>
-      <c r="C47" s="14">
+      <c r="C47" s="7">
         <v>1369616339</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="16" customHeight="1">
-      <c r="A48" s="13" t="s">
+      <c r="A48" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B48" s="15">
+      <c r="B48" s="8">
         <v>34035</v>
       </c>
-      <c r="C48" s="14">
+      <c r="C48" s="7">
         <v>6542045089</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="16" customHeight="1">
-      <c r="A49" s="13" t="s">
+      <c r="A49" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B49" s="15">
+      <c r="B49" s="8">
         <v>134737</v>
       </c>
-      <c r="C49" s="14">
+      <c r="C49" s="7">
         <v>28483710273</v>
       </c>
     </row>
@@ -1278,86 +1277,86 @@
       </c>
     </row>
     <row r="51" spans="1:3" ht="16" customHeight="1">
-      <c r="A51" s="13" t="s">
+      <c r="A51" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B51" s="15">
+      <c r="B51" s="8">
         <v>40371</v>
       </c>
-      <c r="C51" s="14">
+      <c r="C51" s="7">
         <v>8721170223</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="16" customHeight="1">
-      <c r="A52" s="13" t="s">
+      <c r="A52" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B52" s="13">
+      <c r="B52" s="6">
         <v>240</v>
       </c>
-      <c r="C52" s="14">
+      <c r="C52" s="7">
         <v>62242612</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="16" customHeight="1">
-      <c r="A53" s="13" t="s">
+      <c r="A53" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B53" s="15">
+      <c r="B53" s="8">
         <v>6983</v>
       </c>
-      <c r="C53" s="14">
+      <c r="C53" s="7">
         <v>1000127478</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="16" customHeight="1">
-      <c r="A54" s="13" t="s">
+      <c r="A54" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B54" s="15">
+      <c r="B54" s="8">
         <v>30421</v>
       </c>
-      <c r="C54" s="14">
+      <c r="C54" s="7">
         <v>6959680159</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="16" customHeight="1">
-      <c r="A55" s="13" t="s">
+      <c r="A55" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B55" s="15">
+      <c r="B55" s="8">
         <v>43395</v>
       </c>
-      <c r="C55" s="14">
+      <c r="C55" s="7">
         <v>8317705842</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="16" customHeight="1">
-      <c r="A56" s="13" t="s">
+      <c r="A56" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B56" s="15">
+      <c r="B56" s="8">
         <v>7861</v>
       </c>
-      <c r="C56" s="14">
+      <c r="C56" s="7">
         <v>1351223328</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="16" customHeight="1">
-      <c r="A57" s="13" t="s">
+      <c r="A57" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B57" s="15">
+      <c r="B57" s="8">
         <v>7618</v>
       </c>
-      <c r="C57" s="14">
+      <c r="C57" s="7">
         <v>837018372</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="16" customHeight="1">
-      <c r="A58" s="13"/>
-      <c r="B58" s="15"/>
-      <c r="C58" s="14"/>
+      <c r="A58" s="6"/>
+      <c r="B58" s="8"/>
+      <c r="C58" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1371,11 +1370,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10DB64E2-34A2-0448-B366-AA673CAA8723}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -1386,222 +1383,143 @@
     <col min="5" max="5" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:5" ht="16" customHeight="1">
+      <c r="A1" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C1" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="E1" s="9" t="s">
+    </row>
+    <row r="2" spans="1:5" ht="16" customHeight="1">
+      <c r="A2" s="11" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="5" t="s">
+      <c r="B2" s="12">
+        <v>1229893</v>
+      </c>
+      <c r="C2" s="13">
+        <v>58321791761</v>
+      </c>
+      <c r="D2" s="14">
+        <v>0.74029999999999996</v>
+      </c>
+      <c r="E2" s="14">
+        <v>0.1704</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="16" customHeight="1">
+      <c r="A3" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="6">
-        <v>1229893</v>
-      </c>
-      <c r="C3" s="7">
-        <v>58321791761</v>
-      </c>
-      <c r="D3" s="8">
-        <v>0.74029999999999996</v>
-      </c>
-      <c r="E3" s="8">
-        <v>0.1704</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="5"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="5" t="s">
+      <c r="B3" s="12">
+        <v>224061</v>
+      </c>
+      <c r="C3" s="13">
+        <v>50926354675</v>
+      </c>
+      <c r="D3" s="14">
+        <v>0.13489999999999999</v>
+      </c>
+      <c r="E3" s="14">
+        <v>0.14879999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="16" customHeight="1">
+      <c r="A4" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="6">
-        <v>224061</v>
-      </c>
-      <c r="C5" s="7">
-        <v>50926354675</v>
-      </c>
-      <c r="D5" s="8">
-        <v>0.13489999999999999</v>
-      </c>
-      <c r="E5" s="8">
-        <v>0.14879999999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="5"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="5" t="s">
+      <c r="B4" s="12">
+        <v>140197</v>
+      </c>
+      <c r="C4" s="13">
+        <v>80628410796</v>
+      </c>
+      <c r="D4" s="14">
+        <v>8.4400000000000003E-2</v>
+      </c>
+      <c r="E4" s="14">
+        <v>0.2356</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="16" customHeight="1">
+      <c r="A5" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="B7" s="6">
-        <v>140197</v>
-      </c>
-      <c r="C7" s="7">
-        <v>80628410796</v>
-      </c>
-      <c r="D7" s="8">
-        <v>8.4400000000000003E-2</v>
-      </c>
-      <c r="E7" s="8">
-        <v>0.2356</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="5" t="s">
+      <c r="B5" s="12">
+        <v>41238</v>
+      </c>
+      <c r="C5" s="13">
+        <v>57187983464</v>
+      </c>
+      <c r="D5" s="14">
+        <v>2.4799999999999999E-2</v>
+      </c>
+      <c r="E5" s="14">
+        <v>0.1671</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="16" customHeight="1">
+      <c r="A6" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="B9" s="6">
-        <v>41238</v>
-      </c>
-      <c r="C9" s="7">
-        <v>57187983464</v>
-      </c>
-      <c r="D9" s="8">
-        <v>2.4799999999999999E-2</v>
-      </c>
-      <c r="E9" s="8">
-        <v>0.1671</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="5"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="5" t="s">
+      <c r="B6" s="12">
+        <v>21566</v>
+      </c>
+      <c r="C6" s="13">
+        <v>64315474825</v>
+      </c>
+      <c r="D6" s="14">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="E6" s="14">
+        <v>0.18790000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="16" customHeight="1">
+      <c r="A7" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="B11" s="6">
-        <v>21566</v>
-      </c>
-      <c r="C11" s="7">
-        <v>64315474825</v>
-      </c>
-      <c r="D11" s="8">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="E11" s="8">
-        <v>0.18790000000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="5"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B13" s="6">
+      <c r="B7" s="12">
         <v>4412</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C7" s="13">
         <v>30897983582</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D7" s="14">
         <v>2.7000000000000001E-3</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E7" s="14">
         <v>9.0300000000000005E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="5"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
+    <row r="8" spans="1:5" ht="16" customHeight="1">
+      <c r="A8" s="11"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="35">
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AEC82BD-FC4F-384C-ABF2-E24C01262300}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1612,321 +1530,189 @@
     <col min="4" max="4" width="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:4" ht="16" customHeight="1">
+      <c r="A1" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="16" customHeight="1">
+      <c r="A2" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="4" t="s">
+      <c r="B2" s="12">
+        <v>177905</v>
+      </c>
+      <c r="C2" s="13">
+        <v>44906538010</v>
+      </c>
+      <c r="D2" s="15">
+        <v>0.13120000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="16" customHeight="1">
+      <c r="A3" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="6">
-        <v>177905</v>
-      </c>
-      <c r="C3" s="7">
-        <v>44906538010</v>
-      </c>
-      <c r="D3" s="11">
-        <v>0.13120000000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="4"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="11"/>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="4" t="s">
+      <c r="B3" s="12">
+        <v>208360</v>
+      </c>
+      <c r="C3" s="13">
+        <v>43294713938</v>
+      </c>
+      <c r="D3" s="15">
+        <v>0.1265</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="16" customHeight="1">
+      <c r="A4" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="B5" s="6">
-        <v>208360</v>
-      </c>
-      <c r="C5" s="7">
-        <v>43294713938</v>
-      </c>
-      <c r="D5" s="11">
-        <v>0.1265</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="4"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="11"/>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="4" t="s">
+      <c r="B4" s="12">
+        <v>108863</v>
+      </c>
+      <c r="C4" s="13">
+        <v>40922240021</v>
+      </c>
+      <c r="D4" s="15">
+        <v>0.1196</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="16" customHeight="1">
+      <c r="A5" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B7" s="6">
-        <v>108863</v>
-      </c>
-      <c r="C7" s="7">
-        <v>40922240021</v>
-      </c>
-      <c r="D7" s="11">
-        <v>0.1196</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="4"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="11"/>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="4" t="s">
+      <c r="B5" s="12">
+        <v>183542</v>
+      </c>
+      <c r="C5" s="13">
+        <v>39892493481</v>
+      </c>
+      <c r="D5" s="15">
+        <v>0.11650000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="16" customHeight="1">
+      <c r="A6" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="B9" s="6">
-        <v>183542</v>
-      </c>
-      <c r="C9" s="7">
-        <v>39892493481</v>
-      </c>
-      <c r="D9" s="11">
-        <v>0.11650000000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="4"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="11"/>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="4" t="s">
+      <c r="B6" s="12">
+        <v>161876</v>
+      </c>
+      <c r="C6" s="13">
+        <v>30500417573</v>
+      </c>
+      <c r="D6" s="15">
+        <v>8.9099999999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="16" customHeight="1">
+      <c r="A7" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B11" s="6">
-        <v>161876</v>
-      </c>
-      <c r="C11" s="7">
-        <v>30500417573</v>
-      </c>
-      <c r="D11" s="11">
-        <v>8.9099999999999999E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="4"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="11"/>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="4" t="s">
+      <c r="B7" s="12">
+        <v>186429</v>
+      </c>
+      <c r="C7" s="13">
+        <v>29418369063</v>
+      </c>
+      <c r="D7" s="15">
+        <v>8.5900000000000004E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="16" customHeight="1">
+      <c r="A8" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="6">
-        <v>186429</v>
-      </c>
-      <c r="C13" s="7">
-        <v>29418369063</v>
-      </c>
-      <c r="D13" s="11">
-        <v>8.5900000000000004E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="4"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="11"/>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="4" t="s">
+      <c r="B8" s="12">
+        <v>65078</v>
+      </c>
+      <c r="C8" s="13">
+        <v>19489410472</v>
+      </c>
+      <c r="D8" s="15">
+        <v>5.6899999999999999E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="16" customHeight="1">
+      <c r="A9" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="6">
-        <v>65078</v>
-      </c>
-      <c r="C15" s="7">
-        <v>19489410472</v>
-      </c>
-      <c r="D15" s="11">
-        <v>5.6899999999999999E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="4"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="11"/>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="4" t="s">
+      <c r="B9" s="12">
+        <v>155319</v>
+      </c>
+      <c r="C9" s="13">
+        <v>17707077167</v>
+      </c>
+      <c r="D9" s="15">
+        <v>5.1700000000000003E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="16" customHeight="1">
+      <c r="A10" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B17" s="6">
-        <v>155319</v>
-      </c>
-      <c r="C17" s="7">
-        <v>17707077167</v>
-      </c>
-      <c r="D17" s="11">
-        <v>5.1700000000000003E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="4"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="11"/>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="4" t="s">
+      <c r="B10" s="12">
+        <v>72439</v>
+      </c>
+      <c r="C10" s="13">
+        <v>15285814286</v>
+      </c>
+      <c r="D10" s="15">
+        <v>4.4699999999999997E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="16" customHeight="1">
+      <c r="A11" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="B19" s="6">
-        <v>72439</v>
-      </c>
-      <c r="C19" s="7">
-        <v>15285814286</v>
-      </c>
-      <c r="D19" s="11">
-        <v>4.4699999999999997E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="4"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="11"/>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="4" t="s">
+      <c r="B11" s="12">
+        <v>79784</v>
+      </c>
+      <c r="C11" s="13">
+        <v>10743430227</v>
+      </c>
+      <c r="D11" s="15">
+        <v>3.1399999999999997E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="16" customHeight="1">
+      <c r="A12" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B21" s="6">
-        <v>79784</v>
-      </c>
-      <c r="C21" s="7">
-        <v>10743430227</v>
-      </c>
-      <c r="D21" s="11">
-        <v>3.1399999999999997E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="4"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="11"/>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="4" t="s">
+      <c r="B12" s="12">
+        <v>44415</v>
+      </c>
+      <c r="C12" s="13">
+        <v>10598076231</v>
+      </c>
+      <c r="D12" s="15">
+        <v>3.1E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="16" customHeight="1">
+      <c r="A13" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="B23" s="6">
-        <v>44415</v>
-      </c>
-      <c r="C23" s="7">
-        <v>10598076231</v>
-      </c>
-      <c r="D23" s="11">
-        <v>3.1E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="4"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="11"/>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B25" s="6">
+      <c r="B13" s="12">
         <v>60134</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C13" s="13">
         <v>8177041995</v>
       </c>
-      <c r="D25" s="11">
+      <c r="D13" s="15">
         <v>2.3900000000000001E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="4"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="11"/>
-    </row>
   </sheetData>
-  <mergeCells count="52">
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
states and territories extra cells
</commit_message>
<xml_diff>
--- a/data-stories/COVID-19/PPP-data.xlsx
+++ b/data-stories/COVID-19/PPP-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/philiplindsay/Documents/Classes/Psych/Storytelling/git/data-stories/COVID-19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A37AB3A8-3219-7943-8C02-5A8C4F9A8F31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B1CE49-76BF-6847-8AE0-E3A49E1AF6F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{3A25139B-F7C9-2F40-9F60-A201A3DE4647}"/>
   </bookViews>
@@ -293,7 +293,7 @@
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -320,14 +320,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -349,13 +341,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="6" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="6" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -680,10 +670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF7F6668-622A-1B42-AF25-771D7F2C4ECA}">
-  <dimension ref="A1:H58"/>
+  <dimension ref="A1:C58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -692,576 +682,542 @@
     <col min="3" max="3" width="35" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="34" customHeight="1">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:3" ht="34" customHeight="1">
+      <c r="A1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-    </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1">
-      <c r="A2" s="6" t="s">
+    </row>
+    <row r="2" spans="1:3" ht="15" customHeight="1">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="6">
         <v>4842</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="5">
         <v>921927504</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-    </row>
-    <row r="3" spans="1:8" ht="16" customHeight="1">
-      <c r="A3" s="6" t="s">
+    </row>
+    <row r="3" spans="1:3" ht="16" customHeight="1">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="6">
         <v>27922</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="5">
         <v>4862690120</v>
       </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="3"/>
-    </row>
-    <row r="4" spans="1:8" ht="16" customHeight="1">
-      <c r="A4" s="6" t="s">
+    </row>
+    <row r="4" spans="1:3" ht="16" customHeight="1">
+      <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="6">
         <v>21754</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="5">
         <v>2722726557</v>
       </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="3"/>
-    </row>
-    <row r="5" spans="1:8" ht="16" customHeight="1">
-      <c r="A5" s="6" t="s">
+    </row>
+    <row r="5" spans="1:3" ht="16" customHeight="1">
+      <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="4">
         <v>2</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="5">
         <v>419583</v>
       </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="3"/>
-    </row>
-    <row r="6" spans="1:8" ht="16" customHeight="1">
-      <c r="A6" s="6" t="s">
+    </row>
+    <row r="6" spans="1:3" ht="16" customHeight="1">
+      <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="6">
         <v>19280</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="5">
         <v>4846959062</v>
       </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="3"/>
-    </row>
-    <row r="7" spans="1:8" ht="16" customHeight="1">
-      <c r="A7" s="6" t="s">
+    </row>
+    <row r="7" spans="1:3" ht="16" customHeight="1">
+      <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="6">
         <v>112967</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="5">
         <v>33413693192</v>
       </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="3"/>
-    </row>
-    <row r="8" spans="1:8" ht="16" customHeight="1">
-      <c r="A8" s="6" t="s">
+    </row>
+    <row r="8" spans="1:3" ht="16" customHeight="1">
+      <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="6">
         <v>41635</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="5">
         <v>7392960359</v>
       </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="3"/>
-    </row>
-    <row r="9" spans="1:8" ht="16" customHeight="1">
-      <c r="A9" s="6" t="s">
+    </row>
+    <row r="9" spans="1:3" ht="16" customHeight="1">
+      <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="6">
         <v>18435</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="5">
         <v>4151934451</v>
       </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="3"/>
-    </row>
-    <row r="10" spans="1:8" ht="16" customHeight="1">
-      <c r="A10" s="6" t="s">
+    </row>
+    <row r="10" spans="1:3" ht="16" customHeight="1">
+      <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="6">
         <v>3253</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="5">
         <v>1247218727</v>
       </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="3"/>
-    </row>
-    <row r="11" spans="1:8" ht="16" customHeight="1">
-      <c r="A11" s="6" t="s">
+    </row>
+    <row r="11" spans="1:3" ht="16" customHeight="1">
+      <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="6">
         <v>5171</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="5">
         <v>1090415848</v>
       </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="3"/>
-    </row>
-    <row r="12" spans="1:8" ht="16" customHeight="1">
-      <c r="A12" s="6" t="s">
+    </row>
+    <row r="12" spans="1:3" ht="16" customHeight="1">
+      <c r="A12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="6">
         <v>88997</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="5">
         <v>17863199837</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="16" customHeight="1">
-      <c r="A13" s="6" t="s">
+    <row r="13" spans="1:3" ht="16" customHeight="1">
+      <c r="A13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13" s="6">
         <v>48332</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="5">
         <v>9464475442</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="16" customHeight="1">
-      <c r="A14" s="6" t="s">
+    <row r="14" spans="1:3" ht="16" customHeight="1">
+      <c r="A14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="4">
         <v>508</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="5">
         <v>102418346</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="16" customHeight="1">
-      <c r="A15" s="6" t="s">
+    <row r="15" spans="1:3" ht="16" customHeight="1">
+      <c r="A15" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="8">
+      <c r="B15" s="6">
         <v>11553</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="5">
         <v>2046450982</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="16" customHeight="1">
-      <c r="A16" s="6" t="s">
+    <row r="16" spans="1:3" ht="16" customHeight="1">
+      <c r="A16" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16" s="6">
         <v>29424</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="5">
         <v>4315688444</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="16" customHeight="1">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B17" s="6">
         <v>13627</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="5">
         <v>1850034026</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="16" customHeight="1">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18" s="6">
         <v>69893</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="5">
         <v>15972578071</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="16" customHeight="1">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="8">
+      <c r="B19" s="6">
         <v>35990</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="5">
         <v>7491445351</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="16" customHeight="1">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="8">
+      <c r="B20" s="6">
         <v>26245</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="5">
         <v>4288652108</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="16" customHeight="1">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="8">
+      <c r="B21" s="6">
         <v>23797</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="5">
         <v>4149467684</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="16" customHeight="1">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="8">
+      <c r="B22" s="6">
         <v>26635</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C22" s="5">
         <v>5100534501</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="16" customHeight="1">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="8">
+      <c r="B23" s="6">
         <v>46937</v>
       </c>
-      <c r="C23" s="7">
+      <c r="C23" s="5">
         <v>10360907178</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="16" customHeight="1">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="8">
+      <c r="B24" s="6">
         <v>26068</v>
       </c>
-      <c r="C24" s="7">
+      <c r="C24" s="5">
         <v>6537733687</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="16" customHeight="1">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="8">
+      <c r="B25" s="6">
         <v>14993</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C25" s="5">
         <v>1944425549</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="16" customHeight="1">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="8">
+      <c r="B26" s="6">
         <v>43438</v>
       </c>
-      <c r="C26" s="7">
+      <c r="C26" s="5">
         <v>10381310070</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="16" customHeight="1">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="8">
+      <c r="B27" s="6">
         <v>46383</v>
       </c>
-      <c r="C27" s="7">
+      <c r="C27" s="5">
         <v>9014060040</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="16" customHeight="1">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="8">
+      <c r="B28" s="6">
         <v>46481</v>
       </c>
-      <c r="C28" s="7">
+      <c r="C28" s="5">
         <v>7547822023</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="16" customHeight="1">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="6">
+      <c r="B29" s="4">
         <v>56</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C29" s="5">
         <v>12619835</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="16" customHeight="1">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="8">
+      <c r="B30" s="6">
         <v>20748</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C30" s="5">
         <v>2481000606</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="16" customHeight="1">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="8">
+      <c r="B31" s="6">
         <v>13456</v>
       </c>
-      <c r="C31" s="7">
+      <c r="C31" s="5">
         <v>1470300136</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="16" customHeight="1">
-      <c r="A32" s="6" t="s">
+      <c r="A32" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="8">
+      <c r="B32" s="6">
         <v>39520</v>
       </c>
-      <c r="C32" s="7">
+      <c r="C32" s="5">
         <v>8005752270</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="16" customHeight="1">
-      <c r="A33" s="6" t="s">
+      <c r="A33" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="8">
+      <c r="B33" s="6">
         <v>11002</v>
       </c>
-      <c r="C33" s="7">
+      <c r="C33" s="5">
         <v>1548384035</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="16" customHeight="1">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="8">
+      <c r="B34" s="6">
         <v>23477</v>
       </c>
-      <c r="C34" s="7">
+      <c r="C34" s="5">
         <v>2988890489</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="16" customHeight="1">
-      <c r="A35" s="6" t="s">
+      <c r="A35" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="8">
+      <c r="B35" s="6">
         <v>11582</v>
       </c>
-      <c r="C35" s="7">
+      <c r="C35" s="5">
         <v>2006858477</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="16" customHeight="1">
-      <c r="A36" s="6" t="s">
+      <c r="A36" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="8">
+      <c r="B36" s="6">
         <v>33519</v>
       </c>
-      <c r="C36" s="7">
+      <c r="C36" s="5">
         <v>9527794260</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="16" customHeight="1">
-      <c r="A37" s="6" t="s">
+      <c r="A37" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B37" s="8">
+      <c r="B37" s="6">
         <v>8277</v>
       </c>
-      <c r="C37" s="7">
+      <c r="C37" s="5">
         <v>1424408711</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="16" customHeight="1">
-      <c r="A38" s="6" t="s">
+      <c r="A38" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B38" s="8">
+      <c r="B38" s="6">
         <v>8674</v>
       </c>
-      <c r="C38" s="7">
+      <c r="C38" s="5">
         <v>2013939889</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="16" customHeight="1">
-      <c r="A39" s="6" t="s">
+      <c r="A39" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B39" s="8">
+      <c r="B39" s="6">
         <v>81075</v>
       </c>
-      <c r="C39" s="7">
+      <c r="C39" s="5">
         <v>20345681101</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="16" customHeight="1">
-      <c r="A40" s="6" t="s">
+      <c r="A40" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B40" s="8">
+      <c r="B40" s="6">
         <v>59800</v>
       </c>
-      <c r="C40" s="7">
+      <c r="C40" s="5">
         <v>14108889927</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="16" customHeight="1">
-      <c r="A41" s="6" t="s">
+      <c r="A41" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B41" s="8">
+      <c r="B41" s="6">
         <v>35557</v>
       </c>
-      <c r="C41" s="7">
+      <c r="C41" s="5">
         <v>4615708450</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="16" customHeight="1">
-      <c r="A42" s="6" t="s">
+      <c r="A42" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B42" s="8">
+      <c r="B42" s="6">
         <v>18732</v>
       </c>
-      <c r="C42" s="7">
+      <c r="C42" s="5">
         <v>3806104476</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="16" customHeight="1">
-      <c r="A43" s="6" t="s">
+      <c r="A43" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B43" s="8">
+      <c r="B43" s="6">
         <v>69567</v>
       </c>
-      <c r="C43" s="7">
+      <c r="C43" s="5">
         <v>15697648689</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="16" customHeight="1">
-      <c r="A44" s="6" t="s">
+      <c r="A44" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B44" s="8">
+      <c r="B44" s="6">
         <v>2856</v>
       </c>
-      <c r="C44" s="7">
+      <c r="C44" s="5">
         <v>658573638</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="16" customHeight="1">
-      <c r="A45" s="6" t="s">
+      <c r="A45" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B45" s="8">
+      <c r="B45" s="6">
         <v>7732</v>
       </c>
-      <c r="C45" s="7">
+      <c r="C45" s="5">
         <v>1335777801</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="16" customHeight="1">
-      <c r="A46" s="6" t="s">
+      <c r="A46" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B46" s="8">
+      <c r="B46" s="6">
         <v>22933</v>
       </c>
-      <c r="C46" s="7">
+      <c r="C46" s="5">
         <v>3807578397</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="16" customHeight="1">
-      <c r="A47" s="6" t="s">
+      <c r="A47" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B47" s="8">
+      <c r="B47" s="6">
         <v>11324</v>
       </c>
-      <c r="C47" s="7">
+      <c r="C47" s="5">
         <v>1369616339</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="16" customHeight="1">
-      <c r="A48" s="6" t="s">
+      <c r="A48" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B48" s="8">
+      <c r="B48" s="6">
         <v>34035</v>
       </c>
-      <c r="C48" s="7">
+      <c r="C48" s="5">
         <v>6542045089</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="16" customHeight="1">
-      <c r="A49" s="6" t="s">
+      <c r="A49" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B49" s="8">
+      <c r="B49" s="6">
         <v>134737</v>
       </c>
-      <c r="C49" s="7">
+      <c r="C49" s="5">
         <v>28483710273</v>
       </c>
     </row>
@@ -1277,93 +1233,88 @@
       </c>
     </row>
     <row r="51" spans="1:3" ht="16" customHeight="1">
-      <c r="A51" s="6" t="s">
+      <c r="A51" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B51" s="8">
+      <c r="B51" s="6">
         <v>40371</v>
       </c>
-      <c r="C51" s="7">
+      <c r="C51" s="5">
         <v>8721170223</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="16" customHeight="1">
-      <c r="A52" s="6" t="s">
+      <c r="A52" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B52" s="6">
+      <c r="B52" s="4">
         <v>240</v>
       </c>
-      <c r="C52" s="7">
+      <c r="C52" s="5">
         <v>62242612</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="16" customHeight="1">
-      <c r="A53" s="6" t="s">
+      <c r="A53" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B53" s="8">
+      <c r="B53" s="6">
         <v>6983</v>
       </c>
-      <c r="C53" s="7">
+      <c r="C53" s="5">
         <v>1000127478</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="16" customHeight="1">
-      <c r="A54" s="6" t="s">
+      <c r="A54" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B54" s="8">
+      <c r="B54" s="6">
         <v>30421</v>
       </c>
-      <c r="C54" s="7">
+      <c r="C54" s="5">
         <v>6959680159</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="16" customHeight="1">
-      <c r="A55" s="6" t="s">
+      <c r="A55" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B55" s="8">
+      <c r="B55" s="6">
         <v>43395</v>
       </c>
-      <c r="C55" s="7">
+      <c r="C55" s="5">
         <v>8317705842</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="16" customHeight="1">
-      <c r="A56" s="6" t="s">
+      <c r="A56" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B56" s="8">
+      <c r="B56" s="6">
         <v>7861</v>
       </c>
-      <c r="C56" s="7">
+      <c r="C56" s="5">
         <v>1351223328</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="16" customHeight="1">
-      <c r="A57" s="6" t="s">
+      <c r="A57" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B57" s="8">
+      <c r="B57" s="6">
         <v>7618</v>
       </c>
-      <c r="C57" s="7">
+      <c r="C57" s="5">
         <v>837018372</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="16" customHeight="1">
-      <c r="A58" s="6"/>
-      <c r="B58" s="8"/>
-      <c r="C58" s="7"/>
+      <c r="A58" s="4"/>
+      <c r="B58" s="6"/>
+      <c r="C58" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:H2"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1384,130 +1335,130 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16" customHeight="1">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="8" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="16" customHeight="1">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="12">
+      <c r="B2" s="10">
         <v>1229893</v>
       </c>
-      <c r="C2" s="13">
+      <c r="C2" s="11">
         <v>58321791761</v>
       </c>
-      <c r="D2" s="14">
+      <c r="D2" s="12">
         <v>0.74029999999999996</v>
       </c>
-      <c r="E2" s="14">
+      <c r="E2" s="12">
         <v>0.1704</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16" customHeight="1">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="10">
         <v>224061</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C3" s="11">
         <v>50926354675</v>
       </c>
-      <c r="D3" s="14">
+      <c r="D3" s="12">
         <v>0.13489999999999999</v>
       </c>
-      <c r="E3" s="14">
+      <c r="E3" s="12">
         <v>0.14879999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="16" customHeight="1">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="10">
         <v>140197</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C4" s="11">
         <v>80628410796</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="12">
         <v>8.4400000000000003E-2</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="12">
         <v>0.2356</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="16" customHeight="1">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="10">
         <v>41238</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="11">
         <v>57187983464</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="12">
         <v>2.4799999999999999E-2</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="12">
         <v>0.1671</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16" customHeight="1">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="10">
         <v>21566</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="11">
         <v>64315474825</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="12">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="12">
         <v>0.18790000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16" customHeight="1">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="10">
         <v>4412</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="11">
         <v>30897983582</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="12">
         <v>2.7000000000000001E-3</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="12">
         <v>9.0300000000000005E-2</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="16" customHeight="1">
-      <c r="A8" s="11"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1531,184 +1482,184 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="8" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16" customHeight="1">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="12">
+      <c r="B2" s="10">
         <v>177905</v>
       </c>
-      <c r="C2" s="13">
+      <c r="C2" s="11">
         <v>44906538010</v>
       </c>
-      <c r="D2" s="15">
+      <c r="D2" s="13">
         <v>0.13120000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" customHeight="1">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="10">
         <v>208360</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C3" s="11">
         <v>43294713938</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="13">
         <v>0.1265</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16" customHeight="1">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="10">
         <v>108863</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C4" s="11">
         <v>40922240021</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="13">
         <v>0.1196</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="16" customHeight="1">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="10">
         <v>183542</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="11">
         <v>39892493481</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="13">
         <v>0.11650000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16" customHeight="1">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="10">
         <v>161876</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="11">
         <v>30500417573</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="13">
         <v>8.9099999999999999E-2</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="16" customHeight="1">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="10">
         <v>186429</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="11">
         <v>29418369063</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="13">
         <v>8.5900000000000004E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="16" customHeight="1">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="10">
         <v>65078</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="11">
         <v>19489410472</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="13">
         <v>5.6899999999999999E-2</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="16" customHeight="1">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9" s="10">
         <v>155319</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9" s="11">
         <v>17707077167</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="13">
         <v>5.1700000000000003E-2</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="16" customHeight="1">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10" s="10">
         <v>72439</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="11">
         <v>15285814286</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="13">
         <v>4.4699999999999997E-2</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="16" customHeight="1">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B11" s="10">
         <v>79784</v>
       </c>
-      <c r="C11" s="13">
+      <c r="C11" s="11">
         <v>10743430227</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="13">
         <v>3.1399999999999997E-2</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="16" customHeight="1">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B12" s="12">
+      <c r="B12" s="10">
         <v>44415</v>
       </c>
-      <c r="C12" s="13">
+      <c r="C12" s="11">
         <v>10598076231</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="13">
         <v>3.1E-2</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="16" customHeight="1">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B13" s="12">
+      <c r="B13" s="10">
         <v>60134</v>
       </c>
-      <c r="C13" s="13">
+      <c r="C13" s="11">
         <v>8177041995</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="13">
         <v>2.3900000000000001E-2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
eliminated white space after observations
</commit_message>
<xml_diff>
--- a/data-stories/COVID-19/PPP-data.xlsx
+++ b/data-stories/COVID-19/PPP-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/philiplindsay/Documents/Classes/Psych/Storytelling/git/data-stories/COVID-19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DD429A8-2200-0D45-91D3-FB84EE61C01E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4794AFF-8FEB-BA42-9115-2EF4AACDFF14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{3A25139B-F7C9-2F40-9F60-A201A3DE4647}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" activeTab="2" xr2:uid="{3A25139B-F7C9-2F40-9F60-A201A3DE4647}"/>
   </bookViews>
   <sheets>
     <sheet name="states_and_territories" sheetId="1" r:id="rId1"/>
@@ -35,248 +35,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="83">
-  <si>
-    <t xml:space="preserve">AK </t>
-  </si>
-  <si>
-    <t xml:space="preserve">AL </t>
-  </si>
-  <si>
-    <t xml:space="preserve">AR </t>
-  </si>
-  <si>
-    <t xml:space="preserve">AS </t>
-  </si>
-  <si>
-    <t xml:space="preserve">AZ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CA </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CO </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CT </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DC </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FL </t>
-  </si>
-  <si>
-    <t xml:space="preserve">GA </t>
-  </si>
-  <si>
-    <t xml:space="preserve">GU </t>
-  </si>
-  <si>
-    <t xml:space="preserve">HI </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IA </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="82">
   <si>
     <t>State</t>
   </si>
   <si>
-    <t xml:space="preserve">ID </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IL </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IN </t>
-  </si>
-  <si>
-    <t xml:space="preserve">KS </t>
-  </si>
-  <si>
-    <t xml:space="preserve">KY </t>
-  </si>
-  <si>
-    <t xml:space="preserve">LA </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MA </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MD </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ME </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MI </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MN </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MO </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MP </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MS </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MT </t>
-  </si>
-  <si>
-    <t xml:space="preserve">NC </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ND </t>
-  </si>
-  <si>
-    <t xml:space="preserve">NE </t>
-  </si>
-  <si>
-    <t xml:space="preserve">NH </t>
-  </si>
-  <si>
-    <t xml:space="preserve">NJ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">NM </t>
-  </si>
-  <si>
-    <t xml:space="preserve">NV </t>
-  </si>
-  <si>
-    <t xml:space="preserve">NY </t>
-  </si>
-  <si>
-    <t xml:space="preserve">OH </t>
-  </si>
-  <si>
-    <t xml:space="preserve">OK </t>
-  </si>
-  <si>
-    <t xml:space="preserve">OR </t>
-  </si>
-  <si>
-    <t xml:space="preserve">PA </t>
-  </si>
-  <si>
-    <t xml:space="preserve">PR </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RI </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SC </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SD </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TN </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TX </t>
-  </si>
-  <si>
-    <t xml:space="preserve">UT </t>
-  </si>
-  <si>
-    <t xml:space="preserve">VA </t>
-  </si>
-  <si>
-    <t xml:space="preserve">VI </t>
-  </si>
-  <si>
-    <t xml:space="preserve">VT </t>
-  </si>
-  <si>
-    <t xml:space="preserve">WA </t>
-  </si>
-  <si>
-    <t xml:space="preserve">WI </t>
-  </si>
-  <si>
-    <t xml:space="preserve">WV </t>
-  </si>
-  <si>
-    <t xml:space="preserve">WY </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Approved Loans </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Approved Dollars </t>
-  </si>
-  <si>
-    <t xml:space="preserve">% of Count </t>
-  </si>
-  <si>
-    <t xml:space="preserve">% of Amount </t>
-  </si>
-  <si>
-    <t xml:space="preserve">$150K and Under </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&gt;$150K - $350K </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&gt;$350K - $1M </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&gt;$1M - $2M </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&gt;$2M - $5M </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&gt;$5M </t>
-  </si>
-  <si>
-    <t xml:space="preserve">NAICS Subsector Description </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Construction </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Professional, Scientific, and Technical Services </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manufacturing </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Health Care and Social Assistance </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Accommodation and Food Services </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Retail Trade </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wholesale Trade </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other Services (except Public Administration) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Administrative and Support and Waste Management and Remediation Services </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Real Estate and Rental and Leasing </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transportation and Warehousing </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Finance and Insurance </t>
-  </si>
-  <si>
     <t>Approved Loans</t>
   </si>
   <si>
@@ -284,6 +47,240 @@
   </si>
   <si>
     <t>Approved Amounts</t>
+  </si>
+  <si>
+    <t>AK</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
+    <t>AS</t>
+  </si>
+  <si>
+    <t>AZ</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>CT</t>
+  </si>
+  <si>
+    <t>DC</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>FL</t>
+  </si>
+  <si>
+    <t>GA</t>
+  </si>
+  <si>
+    <t>GU</t>
+  </si>
+  <si>
+    <t>HI</t>
+  </si>
+  <si>
+    <t>IA</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>IL</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>KS</t>
+  </si>
+  <si>
+    <t>KY</t>
+  </si>
+  <si>
+    <t>LA</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>MD</t>
+  </si>
+  <si>
+    <t>ME</t>
+  </si>
+  <si>
+    <t>MI</t>
+  </si>
+  <si>
+    <t>MN</t>
+  </si>
+  <si>
+    <t>MO</t>
+  </si>
+  <si>
+    <t>MP</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>MT</t>
+  </si>
+  <si>
+    <t>NC</t>
+  </si>
+  <si>
+    <t>ND</t>
+  </si>
+  <si>
+    <t>NE</t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
+    <t>NJ</t>
+  </si>
+  <si>
+    <t>NM</t>
+  </si>
+  <si>
+    <t>NV</t>
+  </si>
+  <si>
+    <t>NY</t>
+  </si>
+  <si>
+    <t>OH</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>OR</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>PR</t>
+  </si>
+  <si>
+    <t>RI</t>
+  </si>
+  <si>
+    <t>SC</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>TN</t>
+  </si>
+  <si>
+    <t>TX</t>
+  </si>
+  <si>
+    <t>UT</t>
+  </si>
+  <si>
+    <t>VA</t>
+  </si>
+  <si>
+    <t>VI</t>
+  </si>
+  <si>
+    <t>VT</t>
+  </si>
+  <si>
+    <t>WA</t>
+  </si>
+  <si>
+    <t>WI</t>
+  </si>
+  <si>
+    <t>WV</t>
+  </si>
+  <si>
+    <t>WY</t>
+  </si>
+  <si>
+    <t>&gt;$1M - $2M</t>
+  </si>
+  <si>
+    <t>&gt;$5M</t>
+  </si>
+  <si>
+    <t>$150K and Under</t>
+  </si>
+  <si>
+    <t>&gt;$150K - $350K</t>
+  </si>
+  <si>
+    <t>&gt;$350K - $1M</t>
+  </si>
+  <si>
+    <t>&gt;$2M - $5M</t>
+  </si>
+  <si>
+    <t>Approved Dollars</t>
+  </si>
+  <si>
+    <t>% of Count</t>
+  </si>
+  <si>
+    <t>% of Amount</t>
+  </si>
+  <si>
+    <t>NAICS Subsector Description</t>
+  </si>
+  <si>
+    <t>Construction</t>
+  </si>
+  <si>
+    <t>Professional, Scientific, and Technical Services</t>
+  </si>
+  <si>
+    <t>Manufacturing</t>
+  </si>
+  <si>
+    <t>Health Care and Social Assistance</t>
+  </si>
+  <si>
+    <t>Accommodation and Food Services</t>
+  </si>
+  <si>
+    <t>Retail Trade</t>
+  </si>
+  <si>
+    <t>Wholesale Trade</t>
+  </si>
+  <si>
+    <t>Other Services (except Public Administration)</t>
+  </si>
+  <si>
+    <t>Administrative and Support and Waste Management and Remediation Services</t>
+  </si>
+  <si>
+    <t>Real Estate and Rental and Leasing</t>
+  </si>
+  <si>
+    <t>Transportation and Warehousing</t>
+  </si>
+  <si>
+    <t>Finance and Insurance</t>
   </si>
 </sst>
 </file>
@@ -341,7 +338,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -356,6 +353,7 @@
     <xf numFmtId="6" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="6" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -672,8 +670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF7F6668-622A-1B42-AF25-771D7F2C4ECA}">
   <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:G1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -684,18 +682,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="34" customHeight="1">
       <c r="A1" s="7" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>80</v>
+        <v>1</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15" customHeight="1">
       <c r="A2" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B2" s="6">
         <v>4842</v>
@@ -706,7 +704,7 @@
     </row>
     <row r="3" spans="1:3" ht="16" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B3" s="6">
         <v>27922</v>
@@ -717,7 +715,7 @@
     </row>
     <row r="4" spans="1:3" ht="16" customHeight="1">
       <c r="A4" s="4" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B4" s="6">
         <v>21754</v>
@@ -728,7 +726,7 @@
     </row>
     <row r="5" spans="1:3" ht="16" customHeight="1">
       <c r="A5" s="4" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B5" s="4">
         <v>2</v>
@@ -739,7 +737,7 @@
     </row>
     <row r="6" spans="1:3" ht="16" customHeight="1">
       <c r="A6" s="4" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B6" s="6">
         <v>19280</v>
@@ -750,18 +748,18 @@
     </row>
     <row r="7" spans="1:3" ht="16" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B7" s="6">
         <v>112967</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="14">
         <v>33413693192</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="16" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B8" s="6">
         <v>41635</v>
@@ -772,7 +770,7 @@
     </row>
     <row r="9" spans="1:3" ht="16" customHeight="1">
       <c r="A9" s="4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B9" s="6">
         <v>18435</v>
@@ -783,7 +781,7 @@
     </row>
     <row r="10" spans="1:3" ht="16" customHeight="1">
       <c r="A10" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B10" s="6">
         <v>3253</v>
@@ -794,7 +792,7 @@
     </row>
     <row r="11" spans="1:3" ht="16" customHeight="1">
       <c r="A11" s="4" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B11" s="6">
         <v>5171</v>
@@ -805,7 +803,7 @@
     </row>
     <row r="12" spans="1:3" ht="16" customHeight="1">
       <c r="A12" s="4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B12" s="6">
         <v>88997</v>
@@ -816,7 +814,7 @@
     </row>
     <row r="13" spans="1:3" ht="16" customHeight="1">
       <c r="A13" s="4" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B13" s="6">
         <v>48332</v>
@@ -827,7 +825,7 @@
     </row>
     <row r="14" spans="1:3" ht="16" customHeight="1">
       <c r="A14" s="4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B14" s="4">
         <v>508</v>
@@ -838,7 +836,7 @@
     </row>
     <row r="15" spans="1:3" ht="16" customHeight="1">
       <c r="A15" s="4" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B15" s="6">
         <v>11553</v>
@@ -849,7 +847,7 @@
     </row>
     <row r="16" spans="1:3" ht="16" customHeight="1">
       <c r="A16" s="4" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B16" s="6">
         <v>29424</v>
@@ -860,7 +858,7 @@
     </row>
     <row r="17" spans="1:3" ht="16" customHeight="1">
       <c r="A17" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B17" s="6">
         <v>13627</v>
@@ -871,7 +869,7 @@
     </row>
     <row r="18" spans="1:3" ht="16" customHeight="1">
       <c r="A18" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B18" s="6">
         <v>69893</v>
@@ -882,7 +880,7 @@
     </row>
     <row r="19" spans="1:3" ht="16" customHeight="1">
       <c r="A19" s="4" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B19" s="6">
         <v>35990</v>
@@ -893,7 +891,7 @@
     </row>
     <row r="20" spans="1:3" ht="16" customHeight="1">
       <c r="A20" s="4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B20" s="6">
         <v>26245</v>
@@ -904,7 +902,7 @@
     </row>
     <row r="21" spans="1:3" ht="16" customHeight="1">
       <c r="A21" s="4" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B21" s="6">
         <v>23797</v>
@@ -915,7 +913,7 @@
     </row>
     <row r="22" spans="1:3" ht="16" customHeight="1">
       <c r="A22" s="4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B22" s="6">
         <v>26635</v>
@@ -926,7 +924,7 @@
     </row>
     <row r="23" spans="1:3" ht="16" customHeight="1">
       <c r="A23" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B23" s="6">
         <v>46937</v>
@@ -937,7 +935,7 @@
     </row>
     <row r="24" spans="1:3" ht="16" customHeight="1">
       <c r="A24" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B24" s="6">
         <v>26068</v>
@@ -948,7 +946,7 @@
     </row>
     <row r="25" spans="1:3" ht="16" customHeight="1">
       <c r="A25" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B25" s="6">
         <v>14993</v>
@@ -959,7 +957,7 @@
     </row>
     <row r="26" spans="1:3" ht="16" customHeight="1">
       <c r="A26" s="4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B26" s="6">
         <v>43438</v>
@@ -970,7 +968,7 @@
     </row>
     <row r="27" spans="1:3" ht="16" customHeight="1">
       <c r="A27" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B27" s="6">
         <v>46383</v>
@@ -981,7 +979,7 @@
     </row>
     <row r="28" spans="1:3" ht="16" customHeight="1">
       <c r="A28" s="4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B28" s="6">
         <v>46481</v>
@@ -992,7 +990,7 @@
     </row>
     <row r="29" spans="1:3" ht="16" customHeight="1">
       <c r="A29" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B29" s="4">
         <v>56</v>
@@ -1003,7 +1001,7 @@
     </row>
     <row r="30" spans="1:3" ht="16" customHeight="1">
       <c r="A30" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B30" s="6">
         <v>20748</v>
@@ -1014,7 +1012,7 @@
     </row>
     <row r="31" spans="1:3" ht="16" customHeight="1">
       <c r="A31" s="4" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B31" s="6">
         <v>13456</v>
@@ -1025,7 +1023,7 @@
     </row>
     <row r="32" spans="1:3" ht="16" customHeight="1">
       <c r="A32" s="4" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B32" s="6">
         <v>39520</v>
@@ -1036,7 +1034,7 @@
     </row>
     <row r="33" spans="1:3" ht="16" customHeight="1">
       <c r="A33" s="4" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B33" s="6">
         <v>11002</v>
@@ -1047,7 +1045,7 @@
     </row>
     <row r="34" spans="1:3" ht="16" customHeight="1">
       <c r="A34" s="4" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B34" s="6">
         <v>23477</v>
@@ -1058,7 +1056,7 @@
     </row>
     <row r="35" spans="1:3" ht="16" customHeight="1">
       <c r="A35" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B35" s="6">
         <v>11582</v>
@@ -1069,7 +1067,7 @@
     </row>
     <row r="36" spans="1:3" ht="16" customHeight="1">
       <c r="A36" s="4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B36" s="6">
         <v>33519</v>
@@ -1080,7 +1078,7 @@
     </row>
     <row r="37" spans="1:3" ht="16" customHeight="1">
       <c r="A37" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B37" s="6">
         <v>8277</v>
@@ -1091,7 +1089,7 @@
     </row>
     <row r="38" spans="1:3" ht="16" customHeight="1">
       <c r="A38" s="4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B38" s="6">
         <v>8674</v>
@@ -1102,7 +1100,7 @@
     </row>
     <row r="39" spans="1:3" ht="16" customHeight="1">
       <c r="A39" s="4" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B39" s="6">
         <v>81075</v>
@@ -1113,7 +1111,7 @@
     </row>
     <row r="40" spans="1:3" ht="16" customHeight="1">
       <c r="A40" s="4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B40" s="6">
         <v>59800</v>
@@ -1124,7 +1122,7 @@
     </row>
     <row r="41" spans="1:3" ht="16" customHeight="1">
       <c r="A41" s="4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B41" s="6">
         <v>35557</v>
@@ -1135,7 +1133,7 @@
     </row>
     <row r="42" spans="1:3" ht="16" customHeight="1">
       <c r="A42" s="4" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B42" s="6">
         <v>18732</v>
@@ -1146,7 +1144,7 @@
     </row>
     <row r="43" spans="1:3" ht="16" customHeight="1">
       <c r="A43" s="4" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B43" s="6">
         <v>69567</v>
@@ -1157,7 +1155,7 @@
     </row>
     <row r="44" spans="1:3" ht="16" customHeight="1">
       <c r="A44" s="4" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B44" s="6">
         <v>2856</v>
@@ -1168,7 +1166,7 @@
     </row>
     <row r="45" spans="1:3" ht="16" customHeight="1">
       <c r="A45" s="4" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B45" s="6">
         <v>7732</v>
@@ -1179,7 +1177,7 @@
     </row>
     <row r="46" spans="1:3" ht="16" customHeight="1">
       <c r="A46" s="4" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B46" s="6">
         <v>22933</v>
@@ -1190,7 +1188,7 @@
     </row>
     <row r="47" spans="1:3" ht="16" customHeight="1">
       <c r="A47" s="4" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B47" s="6">
         <v>11324</v>
@@ -1201,7 +1199,7 @@
     </row>
     <row r="48" spans="1:3" ht="16" customHeight="1">
       <c r="A48" s="4" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B48" s="6">
         <v>34035</v>
@@ -1212,7 +1210,7 @@
     </row>
     <row r="49" spans="1:3" ht="16" customHeight="1">
       <c r="A49" s="4" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B49" s="6">
         <v>134737</v>
@@ -1223,7 +1221,7 @@
     </row>
     <row r="50" spans="1:3" ht="19">
       <c r="A50" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B50" s="2">
         <v>21257</v>
@@ -1234,7 +1232,7 @@
     </row>
     <row r="51" spans="1:3" ht="16" customHeight="1">
       <c r="A51" s="4" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B51" s="6">
         <v>40371</v>
@@ -1245,7 +1243,7 @@
     </row>
     <row r="52" spans="1:3" ht="16" customHeight="1">
       <c r="A52" s="4" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B52" s="4">
         <v>240</v>
@@ -1256,7 +1254,7 @@
     </row>
     <row r="53" spans="1:3" ht="16" customHeight="1">
       <c r="A53" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B53" s="6">
         <v>6983</v>
@@ -1267,7 +1265,7 @@
     </row>
     <row r="54" spans="1:3" ht="16" customHeight="1">
       <c r="A54" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B54" s="6">
         <v>30421</v>
@@ -1278,7 +1276,7 @@
     </row>
     <row r="55" spans="1:3" ht="16" customHeight="1">
       <c r="A55" s="4" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B55" s="6">
         <v>43395</v>
@@ -1289,7 +1287,7 @@
     </row>
     <row r="56" spans="1:3" ht="16" customHeight="1">
       <c r="A56" s="4" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B56" s="6">
         <v>7861</v>
@@ -1300,7 +1298,7 @@
     </row>
     <row r="57" spans="1:3" ht="16" customHeight="1">
       <c r="A57" s="4" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B57" s="6">
         <v>7618</v>
@@ -1323,7 +1321,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10DB64E2-34A2-0448-B366-AA673CAA8723}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -1336,24 +1336,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="16" customHeight="1">
       <c r="A1" s="8" t="s">
-        <v>81</v>
+        <v>2</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="16" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B2" s="10">
         <v>1229893</v>
@@ -1370,7 +1370,7 @@
     </row>
     <row r="3" spans="1:5" ht="16" customHeight="1">
       <c r="A3" s="9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B3" s="10">
         <v>224061</v>
@@ -1387,7 +1387,7 @@
     </row>
     <row r="4" spans="1:5" ht="16" customHeight="1">
       <c r="A4" s="9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B4" s="10">
         <v>140197</v>
@@ -1404,7 +1404,7 @@
     </row>
     <row r="5" spans="1:5" ht="16" customHeight="1">
       <c r="A5" s="9" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B5" s="10">
         <v>41238</v>
@@ -1438,7 +1438,7 @@
     </row>
     <row r="7" spans="1:5" ht="16" customHeight="1">
       <c r="A7" s="9" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B7" s="10">
         <v>4412</v>
@@ -1469,13 +1469,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AEC82BD-FC4F-384C-ABF2-E24C01262300}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="39.33203125" customWidth="1"/>
+    <col min="1" max="1" width="59.5" customWidth="1"/>
     <col min="2" max="2" width="30.1640625" customWidth="1"/>
     <col min="3" max="3" width="37" customWidth="1"/>
     <col min="4" max="4" width="33" customWidth="1"/>
@@ -1483,21 +1483,21 @@
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1">
       <c r="A1" s="8" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16" customHeight="1">
       <c r="A2" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B2" s="10">
         <v>177905</v>
@@ -1511,7 +1511,7 @@
     </row>
     <row r="3" spans="1:4" ht="16" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B3" s="10">
         <v>208360</v>
@@ -1525,7 +1525,7 @@
     </row>
     <row r="4" spans="1:4" ht="16" customHeight="1">
       <c r="A4" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B4" s="10">
         <v>108863</v>
@@ -1539,7 +1539,7 @@
     </row>
     <row r="5" spans="1:4" ht="16" customHeight="1">
       <c r="A5" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B5" s="10">
         <v>183542</v>
@@ -1553,7 +1553,7 @@
     </row>
     <row r="6" spans="1:4" ht="16" customHeight="1">
       <c r="A6" s="4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B6" s="10">
         <v>161876</v>
@@ -1567,7 +1567,7 @@
     </row>
     <row r="7" spans="1:4" ht="16" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B7" s="10">
         <v>186429</v>
@@ -1581,7 +1581,7 @@
     </row>
     <row r="8" spans="1:4" ht="16" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B8" s="10">
         <v>65078</v>
@@ -1595,7 +1595,7 @@
     </row>
     <row r="9" spans="1:4" ht="16" customHeight="1">
       <c r="A9" s="4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B9" s="10">
         <v>155319</v>
@@ -1609,7 +1609,7 @@
     </row>
     <row r="10" spans="1:4" ht="16" customHeight="1">
       <c r="A10" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B10" s="10">
         <v>72439</v>
@@ -1623,7 +1623,7 @@
     </row>
     <row r="11" spans="1:4" ht="16" customHeight="1">
       <c r="A11" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B11" s="10">
         <v>79784</v>
@@ -1637,7 +1637,7 @@
     </row>
     <row r="12" spans="1:4" ht="16" customHeight="1">
       <c r="A12" s="4" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B12" s="10">
         <v>44415</v>
@@ -1651,7 +1651,7 @@
     </row>
     <row r="13" spans="1:4" ht="16" customHeight="1">
       <c r="A13" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B13" s="10">
         <v>60134</v>

</xml_diff>

<commit_message>
Added new sheets for small businesses by industry and state
</commit_message>
<xml_diff>
--- a/data-stories/COVID-19/PPP-data.xlsx
+++ b/data-stories/COVID-19/PPP-data.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/philiplindsay/Documents/Classes/Psych/Storytelling/git/data-stories/COVID-19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4794AFF-8FEB-BA42-9115-2EF4AACDFF14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4029875A-B3C3-164F-8152-DD9247EBBDA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" activeTab="2" xr2:uid="{3A25139B-F7C9-2F40-9F60-A201A3DE4647}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" activeTab="4" xr2:uid="{3A25139B-F7C9-2F40-9F60-A201A3DE4647}"/>
   </bookViews>
   <sheets>
-    <sheet name="states_and_territories" sheetId="1" r:id="rId1"/>
-    <sheet name="loan_size" sheetId="2" r:id="rId2"/>
-    <sheet name="industry_by_naics_subsector" sheetId="3" r:id="rId3"/>
+    <sheet name="Loans by State" sheetId="1" r:id="rId1"/>
+    <sheet name="Loan Sizes" sheetId="2" r:id="rId2"/>
+    <sheet name="Loans by Industry" sheetId="3" r:id="rId3"/>
+    <sheet name="Small Businesses by State" sheetId="4" r:id="rId4"/>
+    <sheet name="Small Businesses by Industry" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="84">
   <si>
     <t>State</t>
   </si>
@@ -244,9 +246,6 @@
     <t>% of Amount</t>
   </si>
   <si>
-    <t>NAICS Subsector Description</t>
-  </si>
-  <si>
     <t>Construction</t>
   </si>
   <si>
@@ -281,6 +280,15 @@
   </si>
   <si>
     <t>Finance and Insurance</t>
+  </si>
+  <si>
+    <t>Small Businesses</t>
+  </si>
+  <si>
+    <t>Industry</t>
+  </si>
+  <si>
+    <t>Administrative, Support, and Waste Management</t>
   </si>
 </sst>
 </file>
@@ -290,7 +298,7 @@
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -317,6 +325,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -338,7 +352,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -346,6 +360,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="6" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -354,6 +369,9 @@
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="6" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -671,7 +689,7 @@
   <dimension ref="A1:C58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -681,13 +699,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="34" customHeight="1">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="8" t="s">
         <v>3</v>
       </c>
     </row>
@@ -753,7 +771,7 @@
       <c r="B7" s="6">
         <v>112967</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="15">
         <v>33413693192</v>
       </c>
     </row>
@@ -1335,130 +1353,130 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16" customHeight="1">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="9" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="16" customHeight="1">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="11">
         <v>1229893</v>
       </c>
-      <c r="C2" s="11">
+      <c r="C2" s="12">
         <v>58321791761</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="13">
         <v>0.74029999999999996</v>
       </c>
-      <c r="E2" s="12">
+      <c r="E2" s="13">
         <v>0.1704</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16" customHeight="1">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="11">
         <v>224061</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="12">
         <v>50926354675</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="13">
         <v>0.13489999999999999</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="13">
         <v>0.14879999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="16" customHeight="1">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="11">
         <v>140197</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="12">
         <v>80628410796</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="13">
         <v>8.4400000000000003E-2</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="13">
         <v>0.2356</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="16" customHeight="1">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="11">
         <v>41238</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="12">
         <v>57187983464</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="13">
         <v>2.4799999999999999E-2</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="13">
         <v>0.1671</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16" customHeight="1">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="11">
         <v>21566</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="12">
         <v>64315474825</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="13">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="13">
         <v>0.18790000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16" customHeight="1">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="11">
         <v>4412</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="12">
         <v>30897983582</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="13">
         <v>2.7000000000000001E-3</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="13">
         <v>9.0300000000000005E-2</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="16" customHeight="1">
-      <c r="A8" s="9"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1469,8 +1487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AEC82BD-FC4F-384C-ABF2-E24C01262300}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1482,185 +1500,784 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1">
-      <c r="A1" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="B1" s="8" t="s">
+      <c r="A1" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="9" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16" customHeight="1">
       <c r="A2" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B2" s="10">
+        <v>69</v>
+      </c>
+      <c r="B2" s="11">
         <v>177905</v>
       </c>
-      <c r="C2" s="11">
+      <c r="C2" s="12">
         <v>44906538010</v>
       </c>
-      <c r="D2" s="13">
+      <c r="D2" s="14">
         <v>0.13120000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B3" s="10">
+        <v>70</v>
+      </c>
+      <c r="B3" s="11">
         <v>208360</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="12">
         <v>43294713938</v>
       </c>
-      <c r="D3" s="13">
+      <c r="D3" s="14">
         <v>0.1265</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16" customHeight="1">
       <c r="A4" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B4" s="10">
+        <v>71</v>
+      </c>
+      <c r="B4" s="11">
         <v>108863</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="12">
         <v>40922240021</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="14">
         <v>0.1196</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="16" customHeight="1">
       <c r="A5" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B5" s="10">
+        <v>72</v>
+      </c>
+      <c r="B5" s="11">
         <v>183542</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="12">
         <v>39892493481</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="14">
         <v>0.11650000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16" customHeight="1">
       <c r="A6" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B6" s="10">
+        <v>73</v>
+      </c>
+      <c r="B6" s="11">
         <v>161876</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="12">
         <v>30500417573</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="14">
         <v>8.9099999999999999E-2</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="16" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B7" s="10">
+        <v>74</v>
+      </c>
+      <c r="B7" s="11">
         <v>186429</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="12">
         <v>29418369063</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="14">
         <v>8.5900000000000004E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="16" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B8" s="10">
+        <v>75</v>
+      </c>
+      <c r="B8" s="11">
         <v>65078</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="12">
         <v>19489410472</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="14">
         <v>5.6899999999999999E-2</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="16" customHeight="1">
       <c r="A9" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B9" s="10">
+        <v>76</v>
+      </c>
+      <c r="B9" s="11">
         <v>155319</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="12">
         <v>17707077167</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="14">
         <v>5.1700000000000003E-2</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="16" customHeight="1">
       <c r="A10" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B10" s="10">
+        <v>77</v>
+      </c>
+      <c r="B10" s="11">
         <v>72439</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="12">
         <v>15285814286</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="14">
         <v>4.4699999999999997E-2</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="16" customHeight="1">
       <c r="A11" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B11" s="10">
+        <v>78</v>
+      </c>
+      <c r="B11" s="11">
         <v>79784</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="12">
         <v>10743430227</v>
       </c>
-      <c r="D11" s="13">
+      <c r="D11" s="14">
         <v>3.1399999999999997E-2</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="16" customHeight="1">
       <c r="A12" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B12" s="10">
+        <v>79</v>
+      </c>
+      <c r="B12" s="11">
         <v>44415</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="12">
         <v>10598076231</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="14">
         <v>3.1E-2</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="16" customHeight="1">
       <c r="A13" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" s="11">
+        <v>60134</v>
+      </c>
+      <c r="C13" s="12">
+        <v>8177041995</v>
+      </c>
+      <c r="D13" s="14">
+        <v>2.3900000000000001E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7924D13-08C2-3345-9808-B9533871D4E6}">
+  <dimension ref="A1:C57"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="2" max="2" width="23.83203125" style="17" customWidth="1"/>
+    <col min="3" max="3" width="27" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="B13" s="10">
-        <v>60134</v>
-      </c>
-      <c r="C13" s="11">
-        <v>8177041995</v>
-      </c>
-      <c r="D13" s="13">
-        <v>2.3900000000000001E-2</v>
+      <c r="C1" s="8"/>
+    </row>
+    <row r="2" spans="1:3" ht="18">
+      <c r="A2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="7">
+        <v>73354</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="18">
+      <c r="A3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="7">
+        <v>396432</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="18">
+      <c r="A4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="7">
+        <v>571495</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="18">
+      <c r="A5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="7">
+        <v>249907</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="18">
+      <c r="A6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="7">
+        <v>4000000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="18">
+      <c r="A7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="7">
+        <v>630113</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="18">
+      <c r="A8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="7">
+        <v>346950</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="18">
+      <c r="A9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="7">
+        <v>82121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="18">
+      <c r="A10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="7">
+        <v>76083</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="18">
+      <c r="A11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="7">
+        <v>2500000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="18">
+      <c r="A12" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="7">
+        <v>1100000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="18">
+      <c r="A13" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="7">
+        <v>132640</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="18">
+      <c r="A14" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="7">
+        <v>162905</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="18">
+      <c r="A15" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="7">
+        <v>1200000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="18">
+      <c r="A16" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="7">
+        <v>512348</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="18">
+      <c r="A17" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="7">
+        <v>270484</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="18">
+      <c r="A18" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="7">
+        <v>254297</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="18">
+      <c r="A19" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="7">
+        <v>351260</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="18">
+      <c r="A20" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="7">
+        <v>447440</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="18">
+      <c r="A21" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="7">
+        <v>147270</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="18">
+      <c r="A22" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="7">
+        <v>594124</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="18">
+      <c r="A23" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="7">
+        <v>669224</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="18">
+      <c r="A24" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="7">
+        <v>873722</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="18">
+      <c r="A25" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" s="7">
+        <v>520110</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="18">
+      <c r="A26" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="7">
+        <v>257404</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="18">
+      <c r="A27" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="7">
+        <v>532277</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="18">
+      <c r="A28" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="7">
+        <v>120246</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="18">
+      <c r="A29" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="7">
+        <v>176358</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="18">
+      <c r="A30" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" s="7">
+        <v>270079</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="18">
+      <c r="A31" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" s="7">
+        <v>134760</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="18">
+      <c r="A32" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32" s="7">
+        <v>884049</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="18">
+      <c r="A33" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33" s="7">
+        <v>154804</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="18">
+      <c r="A34" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34" s="7">
+        <v>2200000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="18">
+      <c r="A35" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" s="7">
+        <v>913398</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="18">
+      <c r="A36" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" s="7">
+        <v>73142</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="18">
+      <c r="A37" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B37" s="7">
+        <v>949479</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="18">
+      <c r="A38" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B38" s="7">
+        <v>350718</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="18">
+      <c r="A39" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39" s="7">
+        <v>377860</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="18">
+      <c r="A40" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B40" s="7">
+        <v>1100000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="18">
+      <c r="A41" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B41" s="7">
+        <v>101516</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="18">
+      <c r="A42" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B42" s="7">
+        <v>418031</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="18">
+      <c r="A43" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B43" s="7">
+        <v>86550</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="18">
+      <c r="A44" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B44" s="7">
+        <v>603310</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="18">
+      <c r="A45" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B45" s="7">
+        <v>2700000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="18">
+      <c r="A46" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B46" s="7">
+        <v>287803</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="18">
+      <c r="A47" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B47" s="7">
+        <v>77614</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="18">
+      <c r="A48" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B48" s="7">
+        <v>745886</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="18">
+      <c r="A49" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B49" s="7">
+        <v>608956</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="18">
+      <c r="A50" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B50" s="7">
+        <v>113410</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="18">
+      <c r="A51" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B51" s="7">
+        <v>452594</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="18">
+      <c r="A52" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B52" s="7">
+        <v>66653</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="18">
+      <c r="A53" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B53" s="7">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="18">
+      <c r="A54" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B54" s="7">
+        <v>3493</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="18">
+      <c r="A55" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B55" s="7">
+        <v>1757</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="18">
+      <c r="A56" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B56" s="7">
+        <v>43182</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="18">
+      <c r="A57" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B57" s="7">
+        <v>2525</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47F75C5C-FD9B-A546-B43E-FD67BE350860}">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="36.83203125" customWidth="1"/>
+    <col min="2" max="2" width="33" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="18">
+      <c r="A1" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="18">
+      <c r="A2" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="18">
+        <v>3153318</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="18">
+      <c r="A3" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="18">
+        <v>4243655</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="18">
+      <c r="A4" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="18">
+        <v>595271</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="18">
+      <c r="A5" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="18">
+        <v>2611113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="18">
+      <c r="A6" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" s="18">
+        <v>908281</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="18">
+      <c r="A7" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" s="18">
+        <v>2652398</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="18">
+      <c r="A8" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="18">
+        <v>707066</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="18">
+      <c r="A9" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" s="18">
+        <v>4369360</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="18">
+      <c r="A10" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" s="18">
+        <v>2419721</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="18">
+      <c r="A11" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" s="18">
+        <v>2976866</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="18">
+      <c r="A12" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" s="18">
+        <v>2044156</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="18">
+      <c r="A13" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" s="18">
+        <v>953064</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
continuity across rows in the industry sheets
</commit_message>
<xml_diff>
--- a/data-stories/COVID-19/PPP-data.xlsx
+++ b/data-stories/COVID-19/PPP-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/philiplindsay/Documents/Classes/Psych/Storytelling/git/data-stories/COVID-19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4029875A-B3C3-164F-8152-DD9247EBBDA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{560CA545-3024-9F4C-9E86-0E6512F9D626}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" activeTab="4" xr2:uid="{3A25139B-F7C9-2F40-9F60-A201A3DE4647}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" activeTab="2" xr2:uid="{3A25139B-F7C9-2F40-9F60-A201A3DE4647}"/>
   </bookViews>
   <sheets>
     <sheet name="Loans by State" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="83">
   <si>
     <t>State</t>
   </si>
@@ -268,9 +268,6 @@
   </si>
   <si>
     <t>Other Services (except Public Administration)</t>
-  </si>
-  <si>
-    <t>Administrative and Support and Waste Management and Remediation Services</t>
   </si>
   <si>
     <t>Real Estate and Rental and Leasing</t>
@@ -1487,8 +1484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AEC82BD-FC4F-384C-ABF2-E24C01262300}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1501,7 +1498,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1">
       <c r="A1" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>1</v>
@@ -1514,7 +1511,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="16" customHeight="1">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="7" t="s">
         <v>69</v>
       </c>
       <c r="B2" s="11">
@@ -1528,7 +1525,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" customHeight="1">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="7" t="s">
         <v>70</v>
       </c>
       <c r="B3" s="11">
@@ -1542,7 +1539,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="16" customHeight="1">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="7" t="s">
         <v>71</v>
       </c>
       <c r="B4" s="11">
@@ -1556,7 +1553,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="16" customHeight="1">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="7" t="s">
         <v>72</v>
       </c>
       <c r="B5" s="11">
@@ -1570,7 +1567,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="16" customHeight="1">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="7" t="s">
         <v>73</v>
       </c>
       <c r="B6" s="11">
@@ -1584,7 +1581,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="16" customHeight="1">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="7" t="s">
         <v>74</v>
       </c>
       <c r="B7" s="11">
@@ -1598,7 +1595,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="16" customHeight="1">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="7" t="s">
         <v>75</v>
       </c>
       <c r="B8" s="11">
@@ -1612,7 +1609,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="16" customHeight="1">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="7" t="s">
         <v>76</v>
       </c>
       <c r="B9" s="11">
@@ -1626,8 +1623,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="16" customHeight="1">
-      <c r="A10" s="4" t="s">
-        <v>77</v>
+      <c r="A10" s="7" t="s">
+        <v>82</v>
       </c>
       <c r="B10" s="11">
         <v>72439</v>
@@ -1640,8 +1637,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="16" customHeight="1">
-      <c r="A11" s="4" t="s">
-        <v>78</v>
+      <c r="A11" s="7" t="s">
+        <v>77</v>
       </c>
       <c r="B11" s="11">
         <v>79784</v>
@@ -1654,8 +1651,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="16" customHeight="1">
-      <c r="A12" s="4" t="s">
-        <v>79</v>
+      <c r="A12" s="7" t="s">
+        <v>78</v>
       </c>
       <c r="B12" s="11">
         <v>44415</v>
@@ -1668,8 +1665,8 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="16" customHeight="1">
-      <c r="A13" s="4" t="s">
-        <v>80</v>
+      <c r="A13" s="7" t="s">
+        <v>79</v>
       </c>
       <c r="B13" s="11">
         <v>60134</v>
@@ -1691,7 +1688,7 @@
   <dimension ref="A1:C57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1705,7 +1702,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C1" s="8"/>
     </row>
@@ -2166,22 +2163,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47F75C5C-FD9B-A546-B43E-FD67BE350860}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A2:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="36.83203125" customWidth="1"/>
+    <col min="1" max="1" width="59" customWidth="1"/>
     <col min="2" max="2" width="33" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18">
       <c r="A1" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="18">
@@ -2250,7 +2247,7 @@
     </row>
     <row r="10" spans="1:2" ht="18">
       <c r="A10" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B10" s="18">
         <v>2419721</v>
@@ -2258,7 +2255,7 @@
     </row>
     <row r="11" spans="1:2" ht="18">
       <c r="A11" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B11" s="18">
         <v>2976866</v>
@@ -2266,7 +2263,7 @@
     </row>
     <row r="12" spans="1:2" ht="18">
       <c r="A12" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B12" s="18">
         <v>2044156</v>
@@ -2274,7 +2271,7 @@
     </row>
     <row r="13" spans="1:2" ht="18">
       <c r="A13" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B13" s="18">
         <v>953064</v>

</xml_diff>

<commit_message>
added unemployment data sheet and manufacturing employment by state
</commit_message>
<xml_diff>
--- a/data-stories/COVID-19/PPP-data.xlsx
+++ b/data-stories/COVID-19/PPP-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/philiplindsay/Documents/Classes/Psych/Storytelling/git/data-stories/COVID-19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{560CA545-3024-9F4C-9E86-0E6512F9D626}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D1564CD-4480-EE40-BD2B-191D656D1649}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" activeTab="2" xr2:uid="{3A25139B-F7C9-2F40-9F60-A201A3DE4647}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" activeTab="5" xr2:uid="{3A25139B-F7C9-2F40-9F60-A201A3DE4647}"/>
   </bookViews>
   <sheets>
     <sheet name="Loans by State" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Loans by Industry" sheetId="3" r:id="rId3"/>
     <sheet name="Small Businesses by State" sheetId="4" r:id="rId4"/>
     <sheet name="Small Businesses by Industry" sheetId="5" r:id="rId5"/>
+    <sheet name="Unemployment" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="84">
   <si>
     <t>State</t>
   </si>
@@ -286,6 +287,9 @@
   </si>
   <si>
     <t>Administrative, Support, and Waste Management</t>
+  </si>
+  <si>
+    <t>March</t>
   </si>
 </sst>
 </file>
@@ -295,7 +299,7 @@
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -328,6 +332,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -349,7 +359,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -369,6 +379,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1484,8 +1496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AEC82BD-FC4F-384C-ABF2-E24C01262300}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1688,7 +1700,7 @@
   <dimension ref="A1:C57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B1" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1704,7 +1716,9 @@
       <c r="B1" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="8"/>
+      <c r="C1" s="8" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="2" spans="1:3" ht="18">
       <c r="A2" s="7" t="s">
@@ -1713,6 +1727,9 @@
       <c r="B2" s="7">
         <v>73354</v>
       </c>
+      <c r="C2" s="18">
+        <v>1578</v>
+      </c>
     </row>
     <row r="3" spans="1:3" ht="18">
       <c r="A3" s="7" t="s">
@@ -1721,6 +1738,9 @@
       <c r="B3" s="7">
         <v>396432</v>
       </c>
+      <c r="C3" s="18">
+        <v>7925</v>
+      </c>
     </row>
     <row r="4" spans="1:3" ht="18">
       <c r="A4" s="7" t="s">
@@ -1729,6 +1749,9 @@
       <c r="B4" s="7">
         <v>571495</v>
       </c>
+      <c r="C4" s="18">
+        <v>11057</v>
+      </c>
     </row>
     <row r="5" spans="1:3" ht="18">
       <c r="A5" s="7" t="s">
@@ -1737,6 +1760,9 @@
       <c r="B5" s="7">
         <v>249907</v>
       </c>
+      <c r="C5" s="18">
+        <v>4798</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="18">
       <c r="A6" s="7" t="s">
@@ -1745,6 +1771,9 @@
       <c r="B6" s="7">
         <v>4000000</v>
       </c>
+      <c r="C6" s="18">
+        <v>81114</v>
+      </c>
     </row>
     <row r="7" spans="1:3" ht="18">
       <c r="A7" s="7" t="s">
@@ -1753,6 +1782,9 @@
       <c r="B7" s="7">
         <v>630113</v>
       </c>
+      <c r="C7" s="18">
+        <v>12267</v>
+      </c>
     </row>
     <row r="8" spans="1:3" ht="18">
       <c r="A8" s="7" t="s">
@@ -1761,6 +1793,9 @@
       <c r="B8" s="7">
         <v>346950</v>
       </c>
+      <c r="C8" s="18">
+        <v>7096</v>
+      </c>
     </row>
     <row r="9" spans="1:3" ht="18">
       <c r="A9" s="7" t="s">
@@ -1769,6 +1804,9 @@
       <c r="B9" s="7">
         <v>82121</v>
       </c>
+      <c r="C9" s="18">
+        <v>1151</v>
+      </c>
     </row>
     <row r="10" spans="1:3" ht="18">
       <c r="A10" s="7" t="s">
@@ -1777,6 +1815,9 @@
       <c r="B10" s="7">
         <v>76083</v>
       </c>
+      <c r="C10" s="7">
+        <v>398</v>
+      </c>
     </row>
     <row r="11" spans="1:3" ht="18">
       <c r="A11" s="7" t="s">
@@ -1785,6 +1826,9 @@
       <c r="B11" s="7">
         <v>2500000</v>
       </c>
+      <c r="C11" s="18">
+        <v>34955</v>
+      </c>
     </row>
     <row r="12" spans="1:3" ht="18">
       <c r="A12" s="7" t="s">
@@ -1793,6 +1837,9 @@
       <c r="B12" s="7">
         <v>1100000</v>
       </c>
+      <c r="C12" s="18">
+        <v>16656</v>
+      </c>
     </row>
     <row r="13" spans="1:3" ht="18">
       <c r="A13" s="7" t="s">
@@ -1801,6 +1848,9 @@
       <c r="B13" s="7">
         <v>132640</v>
       </c>
+      <c r="C13" s="18">
+        <v>2924</v>
+      </c>
     </row>
     <row r="14" spans="1:3" ht="18">
       <c r="A14" s="7" t="s">
@@ -1809,6 +1859,9 @@
       <c r="B14" s="7">
         <v>162905</v>
       </c>
+      <c r="C14" s="18">
+        <v>4467</v>
+      </c>
     </row>
     <row r="15" spans="1:3" ht="18">
       <c r="A15" s="7" t="s">
@@ -1817,6 +1870,9 @@
       <c r="B15" s="7">
         <v>1200000</v>
       </c>
+      <c r="C15" s="18">
+        <v>21858</v>
+      </c>
     </row>
     <row r="16" spans="1:3" ht="18">
       <c r="A16" s="7" t="s">
@@ -1825,333 +1881,459 @@
       <c r="B16" s="7">
         <v>512348</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="18">
+      <c r="C16" s="18">
+        <v>13512</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="18">
       <c r="A17" s="7" t="s">
         <v>18</v>
       </c>
       <c r="B17" s="7">
         <v>270484</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="18">
+      <c r="C17" s="18">
+        <v>5703</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="18">
       <c r="A18" s="7" t="s">
         <v>22</v>
       </c>
       <c r="B18" s="7">
         <v>254297</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="18">
+      <c r="C18" s="18">
+        <v>5135</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="18">
       <c r="A19" s="7" t="s">
         <v>23</v>
       </c>
       <c r="B19" s="7">
         <v>351260</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="18">
+      <c r="C19" s="18">
+        <v>6700</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="18">
       <c r="A20" s="7" t="s">
         <v>24</v>
       </c>
       <c r="B20" s="7">
         <v>447440</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="18">
+      <c r="C20" s="18">
+        <v>7123</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="18">
       <c r="A21" s="7" t="s">
         <v>27</v>
       </c>
       <c r="B21" s="7">
         <v>147270</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" ht="18">
+      <c r="C21" s="18">
+        <v>3986</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="18">
       <c r="A22" s="7" t="s">
         <v>26</v>
       </c>
       <c r="B22" s="7">
         <v>594124</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" ht="18">
+      <c r="C22" s="18">
+        <v>7220</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="18">
       <c r="A23" s="7" t="s">
         <v>25</v>
       </c>
       <c r="B23" s="7">
         <v>669224</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" ht="18">
+      <c r="C23" s="18">
+        <v>11880</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="18">
       <c r="A24" s="7" t="s">
         <v>28</v>
       </c>
       <c r="B24" s="7">
         <v>873722</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" ht="18">
+      <c r="C24" s="18">
+        <v>22726</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="18">
       <c r="A25" s="7" t="s">
         <v>29</v>
       </c>
       <c r="B25" s="7">
         <v>520110</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" ht="18">
+      <c r="C25" s="18">
+        <v>13597</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="18">
       <c r="A26" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B26" s="7">
         <v>257404</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" ht="18">
+      <c r="C26" s="18">
+        <v>4301</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="18">
       <c r="A27" s="7" t="s">
         <v>30</v>
       </c>
       <c r="B27" s="7">
         <v>532277</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" ht="18">
+      <c r="C27" s="18">
+        <v>11056</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="18">
       <c r="A28" s="7" t="s">
         <v>33</v>
       </c>
       <c r="B28" s="7">
         <v>120246</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" ht="18">
+      <c r="C28" s="18">
+        <v>3304</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="18">
       <c r="A29" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B29" s="7">
         <v>176358</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" ht="18">
+      <c r="C29" s="18">
+        <v>2966</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="18">
       <c r="A30" s="7" t="s">
         <v>40</v>
       </c>
       <c r="B30" s="7">
         <v>270079</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" ht="18">
+      <c r="C30" s="18">
+        <v>4210</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="18">
       <c r="A31" s="7" t="s">
         <v>37</v>
       </c>
       <c r="B31" s="7">
         <v>134760</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" ht="18">
+      <c r="C31" s="18">
+        <v>3752</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="18">
       <c r="A32" s="7" t="s">
         <v>38</v>
       </c>
       <c r="B32" s="7">
         <v>884049</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" ht="18">
+      <c r="C32" s="18">
+        <v>13545</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="18">
       <c r="A33" s="7" t="s">
         <v>39</v>
       </c>
       <c r="B33" s="7">
         <v>154804</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" ht="18">
+      <c r="C33" s="18">
+        <v>4097</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="18">
       <c r="A34" s="7" t="s">
         <v>41</v>
       </c>
       <c r="B34" s="7">
         <v>2200000</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" ht="18">
+      <c r="C34" s="18">
+        <v>32780</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="18">
       <c r="A35" s="7" t="s">
         <v>34</v>
       </c>
       <c r="B35" s="7">
         <v>913398</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" ht="18">
+      <c r="C35" s="18">
+        <v>17812</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="18">
       <c r="A36" s="7" t="s">
         <v>35</v>
       </c>
       <c r="B36" s="7">
         <v>73142</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" ht="18">
+      <c r="C36" s="18">
+        <v>1239</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="18">
       <c r="A37" s="7" t="s">
         <v>42</v>
       </c>
       <c r="B37" s="7">
         <v>949479</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" ht="18">
+      <c r="C37" s="18">
+        <v>24776</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="18">
       <c r="A38" s="7" t="s">
         <v>43</v>
       </c>
       <c r="B38" s="7">
         <v>350718</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" ht="18">
+      <c r="C38" s="18">
+        <v>6784</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="18">
       <c r="A39" s="7" t="s">
         <v>44</v>
       </c>
       <c r="B39" s="7">
         <v>377860</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" ht="18">
+      <c r="C39" s="18">
+        <v>12447</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="18">
       <c r="A40" s="7" t="s">
         <v>45</v>
       </c>
       <c r="B40" s="7">
         <v>1100000</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" ht="18">
+      <c r="C40" s="18">
+        <v>25713</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="18">
       <c r="A41" s="7" t="s">
         <v>47</v>
       </c>
       <c r="B41" s="7">
         <v>101516</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" ht="18">
+      <c r="C41" s="18">
+        <v>2431</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="18">
       <c r="A42" s="7" t="s">
         <v>48</v>
       </c>
       <c r="B42" s="7">
         <v>418031</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" ht="18">
+      <c r="C42" s="18">
+        <v>7352</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="18">
       <c r="A43" s="7" t="s">
         <v>49</v>
       </c>
       <c r="B43" s="7">
         <v>86550</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" ht="18">
+      <c r="C43" s="18">
+        <v>1853</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="18">
       <c r="A44" s="7" t="s">
         <v>50</v>
       </c>
       <c r="B44" s="7">
         <v>603310</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" ht="18">
+      <c r="C44" s="18">
+        <v>11093</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="18">
       <c r="A45" s="7" t="s">
         <v>51</v>
       </c>
       <c r="B45" s="7">
         <v>2700000</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" ht="18">
+      <c r="C45" s="18">
+        <v>49918</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="18">
       <c r="A46" s="7" t="s">
         <v>52</v>
       </c>
       <c r="B46" s="7">
         <v>287803</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" ht="18">
+      <c r="C46" s="18">
+        <v>7254</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="18">
       <c r="A47" s="7" t="s">
         <v>55</v>
       </c>
       <c r="B47" s="7">
         <v>77614</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" ht="18">
+      <c r="C47" s="18">
+        <v>2833</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="18">
       <c r="A48" s="7" t="s">
         <v>53</v>
       </c>
       <c r="B48" s="7">
         <v>745886</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" ht="18">
+      <c r="C48" s="18">
+        <v>10356</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="18">
       <c r="A49" s="7" t="s">
         <v>56</v>
       </c>
       <c r="B49" s="7">
         <v>608956</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" ht="18">
+      <c r="C49" s="18">
+        <v>15045</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="18">
       <c r="A50" s="7" t="s">
         <v>58</v>
       </c>
       <c r="B50" s="7">
         <v>113410</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" ht="18">
+      <c r="C50" s="18">
+        <v>2145</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="18">
       <c r="A51" s="7" t="s">
         <v>57</v>
       </c>
       <c r="B51" s="7">
         <v>452594</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" ht="18">
+      <c r="C51" s="18">
+        <v>14448</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="18">
       <c r="A52" s="7" t="s">
         <v>59</v>
       </c>
       <c r="B52" s="7">
         <v>66653</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" ht="18">
+      <c r="C52" s="18">
+        <v>1448</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="18">
       <c r="A53" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B53" s="7">
         <v>502</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" ht="18">
+      <c r="C53" s="7">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="18">
       <c r="A54" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B54" s="7">
         <v>3493</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" ht="18">
+      <c r="C54" s="18">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="18">
       <c r="A55" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B55" s="7">
         <v>1757</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" ht="18">
+      <c r="C55" s="7">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="18">
       <c r="A56" s="7" t="s">
         <v>46</v>
       </c>
       <c r="B56" s="7">
         <v>43182</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" ht="18">
+      <c r="C56" s="18">
+        <v>1703</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="18">
       <c r="A57" s="7" t="s">
         <v>54</v>
       </c>
       <c r="B57" s="7">
         <v>2525</v>
+      </c>
+      <c r="C57" s="7">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -2164,7 +2346,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A2:A13"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2280,4 +2462,439 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94A56ABE-54C0-AB40-BC38-DE37350D56E1}">
+  <dimension ref="A1:B52"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="21.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="18">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="19">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="20">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="19">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="20">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="19">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="20">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="19">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="20">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="19">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="20">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="19">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="20">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="19">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="20">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="19">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="20">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="19">
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="20">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="19">
+      <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="20">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="19">
+      <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="20">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="19">
+      <c r="A13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="20">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="19">
+      <c r="A14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="20">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="19">
+      <c r="A15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="20">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="19">
+      <c r="A16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="20">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="19">
+      <c r="A17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="20">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="19">
+      <c r="A18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="20">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="19">
+      <c r="A19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="20">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="19">
+      <c r="A20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="20">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="19">
+      <c r="A21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="20">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="19">
+      <c r="A22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="20">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="19">
+      <c r="A23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="20">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="19">
+      <c r="A24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="20">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="19">
+      <c r="A25" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" s="20">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="19">
+      <c r="A26" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="20">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="19">
+      <c r="A27" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="20">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="19">
+      <c r="A28" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="20">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="19">
+      <c r="A29" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="20">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="19">
+      <c r="A30" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" s="20">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="19">
+      <c r="A31" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" s="20">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="19">
+      <c r="A32" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32" s="20">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="19">
+      <c r="A33" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33" s="20">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="19">
+      <c r="A34" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34" s="20">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="19">
+      <c r="A35" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" s="20">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="19">
+      <c r="A36" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" s="20">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="19">
+      <c r="A37" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B37" s="20">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="19">
+      <c r="A38" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B38" s="20">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="19">
+      <c r="A39" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39" s="20">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="19">
+      <c r="A40" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B40" s="20">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="19">
+      <c r="A41" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B41" s="20">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="19">
+      <c r="A42" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B42" s="20">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="19">
+      <c r="A43" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B43" s="20">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="19">
+      <c r="A44" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B44" s="20">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="19">
+      <c r="A45" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B45" s="20">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="19">
+      <c r="A46" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B46" s="20">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="19">
+      <c r="A47" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B47" s="20">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="19">
+      <c r="A48" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B48" s="20">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="19">
+      <c r="A49" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B49" s="20">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="19">
+      <c r="A50" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B50" s="20">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="19">
+      <c r="A51" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B51" s="20">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="19">
+      <c r="A52" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B52" s="20">
+        <v>3.7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added Jan. unemployment data
</commit_message>
<xml_diff>
--- a/data-stories/COVID-19/PPP-data.xlsx
+++ b/data-stories/COVID-19/PPP-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/philiplindsay/Documents/Classes/Psych/Storytelling/git/data-stories/COVID-19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D1564CD-4480-EE40-BD2B-191D656D1649}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE55C401-48D8-0340-A98A-EFFE50CB3615}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" activeTab="5" xr2:uid="{3A25139B-F7C9-2F40-9F60-A201A3DE4647}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="85">
   <si>
     <t>State</t>
   </si>
@@ -290,6 +290,9 @@
   </si>
   <si>
     <t>March</t>
+  </si>
+  <si>
+    <t>January</t>
   </si>
 </sst>
 </file>
@@ -1700,7 +1703,7 @@
   <dimension ref="A1:C57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:B1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2466,433 +2469,646 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94A56ABE-54C0-AB40-BC38-DE37350D56E1}">
-  <dimension ref="A1:B52"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="15.33203125" customWidth="1"/>
     <col min="2" max="2" width="21.83203125" customWidth="1"/>
+    <col min="3" max="3" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18">
+    <row r="1" spans="1:4" ht="18">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="19" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="19">
+      <c r="C1" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" s="7"/>
+    </row>
+    <row r="2" spans="1:4" ht="19">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="20">
         <v>5.6</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="19">
+      <c r="C2" s="20">
+        <v>6</v>
+      </c>
+      <c r="D2" s="7"/>
+    </row>
+    <row r="3" spans="1:4" ht="19">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="20">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="19">
+      <c r="C3" s="20">
+        <v>2.7</v>
+      </c>
+      <c r="D3" s="7"/>
+    </row>
+    <row r="4" spans="1:4" ht="19">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="20">
         <v>5.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="19">
+      <c r="C4" s="20">
+        <v>4.5</v>
+      </c>
+      <c r="D4" s="7"/>
+    </row>
+    <row r="5" spans="1:4" ht="19">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="20">
         <v>4.8</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="19">
+      <c r="C5" s="20">
+        <v>3.5</v>
+      </c>
+      <c r="D5" s="7"/>
+    </row>
+    <row r="6" spans="1:4" ht="19">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="20">
         <v>5.3</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="19">
+      <c r="C6" s="20">
+        <v>3.9</v>
+      </c>
+      <c r="D6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" ht="19">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="20">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="19">
+      <c r="C7" s="20">
+        <v>2.5</v>
+      </c>
+      <c r="D7" s="7"/>
+    </row>
+    <row r="8" spans="1:4" ht="19">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="20">
         <v>3.7</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="19">
+      <c r="C8" s="20">
+        <v>3.7</v>
+      </c>
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" spans="1:4" ht="19">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="20">
         <v>5.0999999999999996</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="19">
+      <c r="C9" s="20">
+        <v>4</v>
+      </c>
+      <c r="D9" s="7"/>
+    </row>
+    <row r="10" spans="1:4" ht="19">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="20">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" ht="19">
+      <c r="C10" s="20">
+        <v>5.2</v>
+      </c>
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" spans="1:4" ht="19">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="20">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" ht="19">
+      <c r="C11" s="20">
+        <v>2.8</v>
+      </c>
+      <c r="D11" s="7"/>
+    </row>
+    <row r="12" spans="1:4" ht="19">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="20">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" ht="19">
+      <c r="C12" s="20">
+        <v>3.1</v>
+      </c>
+      <c r="D12" s="7"/>
+    </row>
+    <row r="13" spans="1:4" ht="19">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B13" s="20">
         <v>2.6</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" ht="19">
+      <c r="C13" s="20">
+        <v>2.7</v>
+      </c>
+      <c r="D13" s="7"/>
+    </row>
+    <row r="14" spans="1:4" ht="19">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="20">
         <v>2.6</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" ht="19">
+      <c r="C14" s="20">
+        <v>2.8</v>
+      </c>
+      <c r="D14" s="7"/>
+    </row>
+    <row r="15" spans="1:4" ht="19">
       <c r="A15" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="20">
         <v>4.5999999999999996</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" ht="19">
+      <c r="C15" s="20">
+        <v>3.5</v>
+      </c>
+      <c r="D15" s="7"/>
+    </row>
+    <row r="16" spans="1:4" ht="19">
       <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B16" s="20">
         <v>3.2</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="19">
+      <c r="C16" s="20">
+        <v>3.1</v>
+      </c>
+      <c r="D16" s="7"/>
+    </row>
+    <row r="17" spans="1:4" ht="19">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B17" s="20">
         <v>3.7</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="19">
+      <c r="C17" s="20">
+        <v>2.8</v>
+      </c>
+      <c r="D17" s="7"/>
+    </row>
+    <row r="18" spans="1:4" ht="19">
       <c r="A18" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B18" s="20">
         <v>3.1</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="19">
+      <c r="C18" s="20">
+        <v>3.1</v>
+      </c>
+      <c r="D18" s="7"/>
+    </row>
+    <row r="19" spans="1:4" ht="19">
       <c r="A19" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B19" s="20">
         <v>5.8</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="19">
+      <c r="C19" s="20">
+        <v>4.3</v>
+      </c>
+      <c r="D19" s="7"/>
+    </row>
+    <row r="20" spans="1:4" ht="19">
       <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B20" s="20">
         <v>6.1</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="19">
+      <c r="C20" s="20">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D20" s="7"/>
+    </row>
+    <row r="21" spans="1:4" ht="19">
       <c r="A21" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B21" s="20">
         <v>3.2</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" ht="19">
+      <c r="C21" s="20">
+        <v>3.1</v>
+      </c>
+      <c r="D21" s="7"/>
+    </row>
+    <row r="22" spans="1:4" ht="19">
       <c r="A22" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B22" s="20">
         <v>3.3</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" ht="19">
+      <c r="C22" s="20">
+        <v>3.3</v>
+      </c>
+      <c r="D22" s="7"/>
+    </row>
+    <row r="23" spans="1:4" ht="19">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B23" s="20">
         <v>2.9</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" ht="19">
+      <c r="C23" s="20">
+        <v>2.8</v>
+      </c>
+      <c r="D23" s="7"/>
+    </row>
+    <row r="24" spans="1:4" ht="19">
       <c r="A24" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B24" s="20">
         <v>4.0999999999999996</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" ht="19">
+      <c r="C24" s="20">
+        <v>3.8</v>
+      </c>
+      <c r="D24" s="7"/>
+    </row>
+    <row r="25" spans="1:4" ht="19">
       <c r="A25" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B25" s="20">
         <v>3.1</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" ht="19">
+      <c r="C25" s="20">
+        <v>3.2</v>
+      </c>
+      <c r="D25" s="7"/>
+    </row>
+    <row r="26" spans="1:4" ht="19">
       <c r="A26" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B26" s="20">
         <v>5.3</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" ht="19">
+      <c r="C26" s="20">
+        <v>5.5</v>
+      </c>
+      <c r="D26" s="7"/>
+    </row>
+    <row r="27" spans="1:4" ht="19">
       <c r="A27" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B27" s="20">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" ht="19">
+      <c r="C27" s="20">
+        <v>3.5</v>
+      </c>
+      <c r="D27" s="7"/>
+    </row>
+    <row r="28" spans="1:4" ht="19">
       <c r="A28" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B28" s="20">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" ht="19">
+      <c r="C28" s="20">
+        <v>3.5</v>
+      </c>
+      <c r="D28" s="7"/>
+    </row>
+    <row r="29" spans="1:4" ht="19">
       <c r="A29" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B29" s="20">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" ht="19">
+      <c r="C29" s="20">
+        <v>3.9</v>
+      </c>
+      <c r="D29" s="7"/>
+    </row>
+    <row r="30" spans="1:4" ht="19">
       <c r="A30" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B30" s="20">
         <v>6.3</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" ht="19">
+      <c r="C30" s="20">
+        <v>3.6</v>
+      </c>
+      <c r="D30" s="7"/>
+    </row>
+    <row r="31" spans="1:4" ht="19">
       <c r="A31" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B31" s="20">
         <v>2.6</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" ht="19">
+      <c r="C31" s="20">
+        <v>2.6</v>
+      </c>
+      <c r="D31" s="7"/>
+    </row>
+    <row r="32" spans="1:4" ht="19">
       <c r="A32" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B32" s="20">
         <v>3.8</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" ht="19">
+      <c r="C32" s="20">
+        <v>3.8</v>
+      </c>
+      <c r="D32" s="7"/>
+    </row>
+    <row r="33" spans="1:4" ht="19">
       <c r="A33" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B33" s="20">
         <v>5.9</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" ht="19">
+      <c r="C33" s="20">
+        <v>4.8</v>
+      </c>
+      <c r="D33" s="7"/>
+    </row>
+    <row r="34" spans="1:4" ht="19">
       <c r="A34" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B34" s="20">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" ht="19">
+      <c r="C34" s="20">
+        <v>3.8</v>
+      </c>
+      <c r="D34" s="7"/>
+    </row>
+    <row r="35" spans="1:4" ht="19">
       <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B35" s="20">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" ht="19">
+      <c r="C35" s="20">
+        <v>3.6</v>
+      </c>
+      <c r="D35" s="7"/>
+    </row>
+    <row r="36" spans="1:4" ht="19">
       <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B36" s="20">
         <v>2.2000000000000002</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" ht="19">
+      <c r="C36" s="20">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D36" s="7"/>
+    </row>
+    <row r="37" spans="1:4" ht="19">
       <c r="A37" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B37" s="20">
         <v>5.5</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" ht="19">
+      <c r="C37" s="20">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D37" s="7"/>
+    </row>
+    <row r="38" spans="1:4" ht="19">
       <c r="A38" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B38" s="20">
         <v>3.1</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" ht="19">
+      <c r="C38" s="20">
+        <v>3.3</v>
+      </c>
+      <c r="D38" s="7"/>
+    </row>
+    <row r="39" spans="1:4" ht="19">
       <c r="A39" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B39" s="20">
         <v>3.3</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" ht="19">
+      <c r="C39" s="20">
+        <v>3.3</v>
+      </c>
+      <c r="D39" s="7"/>
+    </row>
+    <row r="40" spans="1:4" ht="19">
       <c r="A40" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B40" s="20">
         <v>6</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" ht="19">
+      <c r="C40" s="20">
+        <v>4.7</v>
+      </c>
+      <c r="D40" s="7"/>
+    </row>
+    <row r="41" spans="1:4" ht="19">
       <c r="A41" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B41" s="20">
         <v>4.5999999999999996</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" ht="19">
+      <c r="C41" s="20">
+        <v>3.1</v>
+      </c>
+      <c r="D41" s="7"/>
+    </row>
+    <row r="42" spans="1:4" ht="19">
       <c r="A42" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B42" s="20">
         <v>2.6</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" ht="19">
+      <c r="C42" s="20">
+        <v>2.4</v>
+      </c>
+      <c r="D42" s="7"/>
+    </row>
+    <row r="43" spans="1:4" ht="19">
       <c r="A43" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B43" s="20">
         <v>3.3</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" ht="19">
+      <c r="C43" s="20">
+        <v>3.4</v>
+      </c>
+      <c r="D43" s="7"/>
+    </row>
+    <row r="44" spans="1:4" ht="19">
       <c r="A44" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B44" s="20">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" ht="19">
+      <c r="C44" s="20">
+        <v>3.3</v>
+      </c>
+      <c r="D44" s="7"/>
+    </row>
+    <row r="45" spans="1:4" ht="19">
       <c r="A45" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B45" s="20">
         <v>4.7</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" ht="19">
+      <c r="C45" s="20">
+        <v>4.5</v>
+      </c>
+      <c r="D45" s="7"/>
+    </row>
+    <row r="46" spans="1:4" ht="19">
       <c r="A46" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B46" s="20">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" ht="19">
+      <c r="C46" s="20">
+        <v>2.5</v>
+      </c>
+      <c r="D46" s="7"/>
+    </row>
+    <row r="47" spans="1:4" ht="19">
       <c r="A47" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B47" s="20">
         <v>3.2</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" ht="19">
+      <c r="C47" s="20">
+        <v>2.4</v>
+      </c>
+      <c r="D47" s="7"/>
+    </row>
+    <row r="48" spans="1:4" ht="19">
       <c r="A48" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B48" s="20">
         <v>3.3</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" ht="19">
+      <c r="C48" s="20">
+        <v>2.7</v>
+      </c>
+      <c r="D48" s="7"/>
+    </row>
+    <row r="49" spans="1:4" ht="19">
       <c r="A49" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B49" s="20">
         <v>5.0999999999999996</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" ht="19">
+      <c r="C49" s="20">
+        <v>3.9</v>
+      </c>
+      <c r="D49" s="7"/>
+    </row>
+    <row r="50" spans="1:4" ht="19">
       <c r="A50" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B50" s="20">
         <v>6.1</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" ht="19">
+      <c r="C50" s="20">
+        <v>5</v>
+      </c>
+      <c r="D50" s="7"/>
+    </row>
+    <row r="51" spans="1:4" ht="19">
       <c r="A51" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B51" s="20">
         <v>3.4</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" ht="19">
+      <c r="C51" s="20">
+        <v>3.5</v>
+      </c>
+      <c r="D51" s="7"/>
+    </row>
+    <row r="52" spans="1:4" ht="19">
       <c r="A52" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B52" s="20">
         <v>3.7</v>
       </c>
+      <c r="C52" s="20">
+        <v>3.7</v>
+      </c>
+      <c r="D52" s="7"/>
+    </row>
+    <row r="53" spans="1:4" ht="18">
+      <c r="C53" s="7"/>
+      <c r="D53" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>